<commit_message>
VLDD : FAST v2
version 18/12/18 9:48
</commit_message>
<xml_diff>
--- a/FAST.xlsx
+++ b/FAST.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12345" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12345"/>
   </bookViews>
   <sheets>
     <sheet name="Global" sheetId="1" r:id="rId1"/>
@@ -68,15 +68,6 @@
     <t>options possiblement ajoutées)</t>
   </si>
   <si>
-    <t>Possèder une source d'</t>
-  </si>
-  <si>
-    <t>énergie propre le rendant</t>
-  </si>
-  <si>
-    <t>indépendant du secteur</t>
-  </si>
-  <si>
     <t>FAST FT3</t>
   </si>
   <si>
@@ -210,6 +201,15 @@
   </si>
   <si>
     <t>répartition du poids</t>
+  </si>
+  <si>
+    <t>Être autonome en énergie</t>
+  </si>
+  <si>
+    <t>et pouvoir se recharger sur le lieu</t>
+  </si>
+  <si>
+    <t>de stockage</t>
   </si>
 </sst>
 </file>
@@ -258,7 +258,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="29">
+  <borders count="27">
     <border>
       <left/>
       <right/>
@@ -287,30 +287,10 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
       <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
       <top/>
       <bottom/>
       <diagonal/>
@@ -562,21 +542,57 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -585,56 +601,15 @@
     <xf numFmtId="49" fontId="1" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="1" fillId="3" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="3" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="1" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="3" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="3" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -647,24 +622,28 @@
     <xf numFmtId="49" fontId="2" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="49" fontId="1" fillId="3" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="49" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="49" fontId="1" fillId="3" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -948,19 +927,19 @@
   <sheetPr>
     <tabColor theme="9" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A1:AM26"/>
+  <dimension ref="A1:AT27"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AH13" sqref="AG13:AH13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="3.5703125" defaultRowHeight="18.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="16384" width="3.5703125" style="47"/>
+    <col min="1" max="16384" width="3.5703125" style="23"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:39" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="45"/>
+    <row r="1" spans="1:45" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="22"/>
       <c r="B1" s="4"/>
       <c r="C1" s="4"/>
       <c r="D1" s="4"/>
@@ -998,9 +977,15 @@
       <c r="AJ1" s="4"/>
       <c r="AK1" s="4"/>
       <c r="AL1" s="4"/>
-      <c r="AM1" s="46"/>
-    </row>
-    <row r="2" spans="1:39" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="AM1" s="4"/>
+      <c r="AN1" s="2"/>
+      <c r="AO1" s="2"/>
+      <c r="AP1" s="2"/>
+      <c r="AQ1" s="2"/>
+      <c r="AR1" s="2"/>
+      <c r="AS1" s="2"/>
+    </row>
+    <row r="2" spans="1:45" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
@@ -1013,20 +998,20 @@
       <c r="J2" s="2"/>
       <c r="K2" s="2"/>
       <c r="L2" s="2"/>
-      <c r="M2" s="7" t="s">
+      <c r="M2" s="29" t="s">
         <v>5</v>
       </c>
-      <c r="N2" s="8"/>
-      <c r="O2" s="10" t="s">
+      <c r="N2" s="30"/>
+      <c r="O2" s="31" t="s">
         <v>6</v>
       </c>
-      <c r="P2" s="10"/>
-      <c r="Q2" s="10"/>
-      <c r="R2" s="10"/>
-      <c r="S2" s="10"/>
-      <c r="T2" s="10"/>
-      <c r="U2" s="10"/>
-      <c r="V2" s="11"/>
+      <c r="P2" s="31"/>
+      <c r="Q2" s="31"/>
+      <c r="R2" s="31"/>
+      <c r="S2" s="31"/>
+      <c r="T2" s="31"/>
+      <c r="U2" s="31"/>
+      <c r="V2" s="32"/>
       <c r="W2" s="2"/>
       <c r="X2" s="2"/>
       <c r="Y2" s="2"/>
@@ -1043,9 +1028,15 @@
       <c r="AJ2" s="2"/>
       <c r="AK2" s="2"/>
       <c r="AL2" s="2"/>
-      <c r="AM2" s="48"/>
-    </row>
-    <row r="3" spans="1:39" ht="18.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="AM2" s="2"/>
+      <c r="AN2" s="2"/>
+      <c r="AO2" s="2"/>
+      <c r="AP2" s="2"/>
+      <c r="AQ2" s="2"/>
+      <c r="AR2" s="2"/>
+      <c r="AS2" s="2"/>
+    </row>
+    <row r="3" spans="1:45" ht="18.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1"/>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
@@ -1057,19 +1048,19 @@
       <c r="I3" s="2"/>
       <c r="J3" s="2"/>
       <c r="K3" s="2"/>
-      <c r="L3" s="49"/>
-      <c r="M3" s="14" t="s">
+      <c r="L3" s="24"/>
+      <c r="M3" s="33" t="s">
         <v>7</v>
       </c>
-      <c r="N3" s="15"/>
-      <c r="O3" s="15"/>
-      <c r="P3" s="15"/>
-      <c r="Q3" s="15"/>
-      <c r="R3" s="15"/>
-      <c r="S3" s="15"/>
-      <c r="T3" s="15"/>
-      <c r="U3" s="15"/>
-      <c r="V3" s="16"/>
+      <c r="N3" s="34"/>
+      <c r="O3" s="34"/>
+      <c r="P3" s="34"/>
+      <c r="Q3" s="34"/>
+      <c r="R3" s="34"/>
+      <c r="S3" s="34"/>
+      <c r="T3" s="34"/>
+      <c r="U3" s="34"/>
+      <c r="V3" s="35"/>
       <c r="W3" s="2"/>
       <c r="X3" s="2"/>
       <c r="Y3" s="2"/>
@@ -1086,9 +1077,15 @@
       <c r="AJ3" s="2"/>
       <c r="AK3" s="2"/>
       <c r="AL3" s="2"/>
-      <c r="AM3" s="48"/>
-    </row>
-    <row r="4" spans="1:39" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="AM3" s="2"/>
+      <c r="AN3" s="2"/>
+      <c r="AO3" s="2"/>
+      <c r="AP3" s="2"/>
+      <c r="AQ3" s="2"/>
+      <c r="AR3" s="2"/>
+      <c r="AS3" s="2"/>
+    </row>
+    <row r="4" spans="1:45" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
@@ -1100,17 +1097,17 @@
       <c r="I4" s="2"/>
       <c r="J4" s="2"/>
       <c r="K4" s="2"/>
-      <c r="L4" s="50"/>
-      <c r="M4" s="22"/>
-      <c r="N4" s="23"/>
-      <c r="O4" s="23"/>
-      <c r="P4" s="23"/>
-      <c r="Q4" s="23"/>
-      <c r="R4" s="23"/>
-      <c r="S4" s="23"/>
-      <c r="T4" s="23"/>
-      <c r="U4" s="23"/>
-      <c r="V4" s="24"/>
+      <c r="L4" s="25"/>
+      <c r="M4" s="36"/>
+      <c r="N4" s="37"/>
+      <c r="O4" s="37"/>
+      <c r="P4" s="37"/>
+      <c r="Q4" s="37"/>
+      <c r="R4" s="37"/>
+      <c r="S4" s="37"/>
+      <c r="T4" s="37"/>
+      <c r="U4" s="37"/>
+      <c r="V4" s="38"/>
       <c r="W4" s="2"/>
       <c r="X4" s="2"/>
       <c r="Y4" s="2"/>
@@ -1127,9 +1124,15 @@
       <c r="AJ4" s="2"/>
       <c r="AK4" s="2"/>
       <c r="AL4" s="2"/>
-      <c r="AM4" s="48"/>
-    </row>
-    <row r="5" spans="1:39" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AM4" s="2"/>
+      <c r="AN4" s="2"/>
+      <c r="AO4" s="2"/>
+      <c r="AP4" s="2"/>
+      <c r="AQ4" s="2"/>
+      <c r="AR4" s="2"/>
+      <c r="AS4" s="2"/>
+    </row>
+    <row r="5" spans="1:45" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1"/>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
@@ -1140,7 +1143,7 @@
       <c r="H5" s="2"/>
       <c r="I5" s="2"/>
       <c r="J5" s="2"/>
-      <c r="K5" s="25"/>
+      <c r="K5" s="11"/>
       <c r="L5" s="2"/>
       <c r="M5" s="2"/>
       <c r="N5" s="2"/>
@@ -1168,9 +1171,15 @@
       <c r="AJ5" s="2"/>
       <c r="AK5" s="2"/>
       <c r="AL5" s="2"/>
-      <c r="AM5" s="48"/>
-    </row>
-    <row r="6" spans="1:39" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AM5" s="2"/>
+      <c r="AN5" s="2"/>
+      <c r="AO5" s="2"/>
+      <c r="AP5" s="2"/>
+      <c r="AQ5" s="2"/>
+      <c r="AR5" s="2"/>
+      <c r="AS5" s="2"/>
+    </row>
+    <row r="6" spans="1:45" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="1"/>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
@@ -1181,7 +1190,7 @@
       <c r="H6" s="2"/>
       <c r="I6" s="2"/>
       <c r="J6" s="2"/>
-      <c r="K6" s="25"/>
+      <c r="K6" s="11"/>
       <c r="L6" s="2"/>
       <c r="M6" s="2"/>
       <c r="N6" s="2"/>
@@ -1209,9 +1218,15 @@
       <c r="AJ6" s="2"/>
       <c r="AK6" s="2"/>
       <c r="AL6" s="2"/>
-      <c r="AM6" s="48"/>
-    </row>
-    <row r="7" spans="1:39" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AM6" s="2"/>
+      <c r="AN6" s="2"/>
+      <c r="AO6" s="2"/>
+      <c r="AP6" s="2"/>
+      <c r="AQ6" s="2"/>
+      <c r="AR6" s="2"/>
+      <c r="AS6" s="2"/>
+    </row>
+    <row r="7" spans="1:45" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="1"/>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
@@ -1222,7 +1237,7 @@
       <c r="H7" s="2"/>
       <c r="I7" s="2"/>
       <c r="J7" s="2"/>
-      <c r="K7" s="25"/>
+      <c r="K7" s="11"/>
       <c r="L7" s="2"/>
       <c r="M7" s="2"/>
       <c r="N7" s="2"/>
@@ -1250,9 +1265,15 @@
       <c r="AJ7" s="2"/>
       <c r="AK7" s="2"/>
       <c r="AL7" s="2"/>
-      <c r="AM7" s="48"/>
-    </row>
-    <row r="8" spans="1:39" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AM7" s="2"/>
+      <c r="AN7" s="2"/>
+      <c r="AO7" s="2"/>
+      <c r="AP7" s="2"/>
+      <c r="AQ7" s="2"/>
+      <c r="AR7" s="2"/>
+      <c r="AS7" s="2"/>
+    </row>
+    <row r="8" spans="1:45" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="1"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
@@ -1264,7 +1285,7 @@
       <c r="I8" s="2"/>
       <c r="J8" s="2"/>
       <c r="K8" s="2"/>
-      <c r="L8" s="50"/>
+      <c r="L8" s="25"/>
       <c r="M8" s="2"/>
       <c r="N8" s="2"/>
       <c r="O8" s="2"/>
@@ -1291,9 +1312,15 @@
       <c r="AJ8" s="2"/>
       <c r="AK8" s="2"/>
       <c r="AL8" s="2"/>
-      <c r="AM8" s="48"/>
-    </row>
-    <row r="9" spans="1:39" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="AM8" s="2"/>
+      <c r="AN8" s="2"/>
+      <c r="AO8" s="2"/>
+      <c r="AP8" s="2"/>
+      <c r="AQ8" s="2"/>
+      <c r="AR8" s="2"/>
+      <c r="AS8" s="2"/>
+    </row>
+    <row r="9" spans="1:45" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
@@ -1305,7 +1332,7 @@
       <c r="I9" s="2"/>
       <c r="J9" s="2"/>
       <c r="K9" s="2"/>
-      <c r="L9" s="50"/>
+      <c r="L9" s="25"/>
       <c r="M9" s="2"/>
       <c r="N9" s="2"/>
       <c r="O9" s="2"/>
@@ -1332,39 +1359,45 @@
       <c r="AJ9" s="2"/>
       <c r="AK9" s="2"/>
       <c r="AL9" s="2"/>
-      <c r="AM9" s="48"/>
-    </row>
-    <row r="10" spans="1:39" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="7" t="s">
+      <c r="AM9" s="2"/>
+      <c r="AN9" s="2"/>
+      <c r="AO9" s="2"/>
+      <c r="AP9" s="2"/>
+      <c r="AQ9" s="2"/>
+      <c r="AR9" s="2"/>
+      <c r="AS9" s="2"/>
+    </row>
+    <row r="10" spans="1:45" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="B10" s="8"/>
-      <c r="C10" s="10" t="s">
+      <c r="B10" s="30"/>
+      <c r="C10" s="31" t="s">
         <v>2</v>
       </c>
-      <c r="D10" s="10"/>
-      <c r="E10" s="10"/>
-      <c r="F10" s="10"/>
-      <c r="G10" s="10"/>
-      <c r="H10" s="10"/>
-      <c r="I10" s="10"/>
-      <c r="J10" s="11"/>
+      <c r="D10" s="31"/>
+      <c r="E10" s="31"/>
+      <c r="F10" s="31"/>
+      <c r="G10" s="31"/>
+      <c r="H10" s="31"/>
+      <c r="I10" s="31"/>
+      <c r="J10" s="32"/>
       <c r="K10" s="2"/>
-      <c r="L10" s="50"/>
-      <c r="M10" s="7" t="s">
+      <c r="L10" s="25"/>
+      <c r="M10" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="N10" s="8"/>
-      <c r="O10" s="10" t="s">
+      <c r="N10" s="30"/>
+      <c r="O10" s="31" t="s">
         <v>10</v>
       </c>
-      <c r="P10" s="10"/>
-      <c r="Q10" s="10"/>
-      <c r="R10" s="10"/>
-      <c r="S10" s="10"/>
-      <c r="T10" s="10"/>
-      <c r="U10" s="10"/>
-      <c r="V10" s="11"/>
+      <c r="P10" s="31"/>
+      <c r="Q10" s="31"/>
+      <c r="R10" s="31"/>
+      <c r="S10" s="31"/>
+      <c r="T10" s="31"/>
+      <c r="U10" s="31"/>
+      <c r="V10" s="32"/>
       <c r="W10" s="2"/>
       <c r="X10" s="2"/>
       <c r="Y10" s="2"/>
@@ -1381,35 +1414,41 @@
       <c r="AJ10" s="2"/>
       <c r="AK10" s="2"/>
       <c r="AL10" s="2"/>
-      <c r="AM10" s="48"/>
-    </row>
-    <row r="11" spans="1:39" ht="18.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="14" t="s">
+      <c r="AM10" s="2"/>
+      <c r="AN10" s="2"/>
+      <c r="AO10" s="2"/>
+      <c r="AP10" s="2"/>
+      <c r="AQ10" s="2"/>
+      <c r="AR10" s="2"/>
+      <c r="AS10" s="2"/>
+    </row>
+    <row r="11" spans="1:45" ht="18.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="33" t="s">
         <v>3</v>
       </c>
-      <c r="B11" s="15"/>
-      <c r="C11" s="15"/>
-      <c r="D11" s="15"/>
-      <c r="E11" s="15"/>
-      <c r="F11" s="15"/>
-      <c r="G11" s="15"/>
-      <c r="H11" s="15"/>
-      <c r="I11" s="15"/>
-      <c r="J11" s="16"/>
-      <c r="K11" s="51"/>
-      <c r="L11" s="49"/>
-      <c r="M11" s="14" t="s">
+      <c r="B11" s="34"/>
+      <c r="C11" s="34"/>
+      <c r="D11" s="34"/>
+      <c r="E11" s="34"/>
+      <c r="F11" s="34"/>
+      <c r="G11" s="34"/>
+      <c r="H11" s="34"/>
+      <c r="I11" s="34"/>
+      <c r="J11" s="35"/>
+      <c r="K11" s="26"/>
+      <c r="L11" s="24"/>
+      <c r="M11" s="33" t="s">
         <v>11</v>
       </c>
-      <c r="N11" s="15"/>
-      <c r="O11" s="15"/>
-      <c r="P11" s="15"/>
-      <c r="Q11" s="15"/>
-      <c r="R11" s="15"/>
-      <c r="S11" s="15"/>
-      <c r="T11" s="15"/>
-      <c r="U11" s="15"/>
-      <c r="V11" s="16"/>
+      <c r="N11" s="34"/>
+      <c r="O11" s="34"/>
+      <c r="P11" s="34"/>
+      <c r="Q11" s="34"/>
+      <c r="R11" s="34"/>
+      <c r="S11" s="34"/>
+      <c r="T11" s="34"/>
+      <c r="U11" s="34"/>
+      <c r="V11" s="35"/>
       <c r="W11" s="2"/>
       <c r="X11" s="2"/>
       <c r="Y11" s="2"/>
@@ -1426,35 +1465,41 @@
       <c r="AJ11" s="2"/>
       <c r="AK11" s="2"/>
       <c r="AL11" s="2"/>
-      <c r="AM11" s="48"/>
-    </row>
-    <row r="12" spans="1:39" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="22" t="s">
+      <c r="AM11" s="2"/>
+      <c r="AN11" s="2"/>
+      <c r="AO11" s="2"/>
+      <c r="AP11" s="2"/>
+      <c r="AQ11" s="2"/>
+      <c r="AR11" s="2"/>
+      <c r="AS11" s="2"/>
+    </row>
+    <row r="12" spans="1:45" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="36" t="s">
         <v>4</v>
       </c>
-      <c r="B12" s="23"/>
-      <c r="C12" s="23"/>
-      <c r="D12" s="23"/>
-      <c r="E12" s="23"/>
-      <c r="F12" s="23"/>
-      <c r="G12" s="23"/>
-      <c r="H12" s="23"/>
-      <c r="I12" s="23"/>
-      <c r="J12" s="24"/>
-      <c r="K12" s="25"/>
+      <c r="B12" s="37"/>
+      <c r="C12" s="37"/>
+      <c r="D12" s="37"/>
+      <c r="E12" s="37"/>
+      <c r="F12" s="37"/>
+      <c r="G12" s="37"/>
+      <c r="H12" s="37"/>
+      <c r="I12" s="37"/>
+      <c r="J12" s="38"/>
+      <c r="K12" s="11"/>
       <c r="L12" s="2"/>
-      <c r="M12" s="22" t="s">
+      <c r="M12" s="36" t="s">
         <v>12</v>
       </c>
-      <c r="N12" s="23"/>
-      <c r="O12" s="23"/>
-      <c r="P12" s="23"/>
-      <c r="Q12" s="23"/>
-      <c r="R12" s="23"/>
-      <c r="S12" s="23"/>
-      <c r="T12" s="23"/>
-      <c r="U12" s="23"/>
-      <c r="V12" s="24"/>
+      <c r="N12" s="37"/>
+      <c r="O12" s="37"/>
+      <c r="P12" s="37"/>
+      <c r="Q12" s="37"/>
+      <c r="R12" s="37"/>
+      <c r="S12" s="37"/>
+      <c r="T12" s="37"/>
+      <c r="U12" s="37"/>
+      <c r="V12" s="38"/>
       <c r="W12" s="2"/>
       <c r="X12" s="2"/>
       <c r="Y12" s="2"/>
@@ -1471,20 +1516,26 @@
       <c r="AJ12" s="2"/>
       <c r="AK12" s="2"/>
       <c r="AL12" s="2"/>
-      <c r="AM12" s="48"/>
-    </row>
-    <row r="13" spans="1:39" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="29"/>
-      <c r="B13" s="29"/>
-      <c r="C13" s="29"/>
-      <c r="D13" s="29"/>
-      <c r="E13" s="29"/>
-      <c r="F13" s="29"/>
-      <c r="G13" s="29"/>
-      <c r="H13" s="29"/>
-      <c r="I13" s="29"/>
+      <c r="AM12" s="2"/>
+      <c r="AN12" s="2"/>
+      <c r="AO12" s="2"/>
+      <c r="AP12" s="2"/>
+      <c r="AQ12" s="2"/>
+      <c r="AR12" s="2"/>
+      <c r="AS12" s="2"/>
+    </row>
+    <row r="13" spans="1:45" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="12"/>
+      <c r="B13" s="12"/>
+      <c r="C13" s="12"/>
+      <c r="D13" s="12"/>
+      <c r="E13" s="12"/>
+      <c r="F13" s="12"/>
+      <c r="G13" s="12"/>
+      <c r="H13" s="12"/>
+      <c r="I13" s="12"/>
       <c r="J13" s="2"/>
-      <c r="K13" s="25"/>
+      <c r="K13" s="11"/>
       <c r="L13" s="2"/>
       <c r="M13" s="2"/>
       <c r="N13" s="2"/>
@@ -1512,20 +1563,26 @@
       <c r="AJ13" s="2"/>
       <c r="AK13" s="2"/>
       <c r="AL13" s="2"/>
-      <c r="AM13" s="48"/>
-    </row>
-    <row r="14" spans="1:39" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="29"/>
-      <c r="B14" s="29"/>
-      <c r="C14" s="29"/>
-      <c r="D14" s="29"/>
-      <c r="E14" s="29"/>
-      <c r="F14" s="29"/>
-      <c r="G14" s="29"/>
-      <c r="H14" s="29"/>
-      <c r="I14" s="29"/>
+      <c r="AM13" s="2"/>
+      <c r="AN13" s="2"/>
+      <c r="AO13" s="2"/>
+      <c r="AP13" s="2"/>
+      <c r="AQ13" s="2"/>
+      <c r="AR13" s="2"/>
+      <c r="AS13" s="2"/>
+    </row>
+    <row r="14" spans="1:45" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="12"/>
+      <c r="B14" s="12"/>
+      <c r="C14" s="12"/>
+      <c r="D14" s="12"/>
+      <c r="E14" s="12"/>
+      <c r="F14" s="12"/>
+      <c r="G14" s="12"/>
+      <c r="H14" s="12"/>
+      <c r="I14" s="12"/>
       <c r="J14" s="2"/>
-      <c r="K14" s="25"/>
+      <c r="K14" s="11"/>
       <c r="L14" s="2"/>
       <c r="M14" s="2"/>
       <c r="N14" s="2"/>
@@ -1553,20 +1610,26 @@
       <c r="AJ14" s="2"/>
       <c r="AK14" s="2"/>
       <c r="AL14" s="2"/>
-      <c r="AM14" s="48"/>
-    </row>
-    <row r="15" spans="1:39" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="29"/>
-      <c r="B15" s="29"/>
-      <c r="C15" s="29"/>
-      <c r="D15" s="29"/>
-      <c r="E15" s="29"/>
-      <c r="F15" s="29"/>
+      <c r="AM14" s="2"/>
+      <c r="AN14" s="2"/>
+      <c r="AO14" s="2"/>
+      <c r="AP14" s="2"/>
+      <c r="AQ14" s="2"/>
+      <c r="AR14" s="2"/>
+      <c r="AS14" s="2"/>
+    </row>
+    <row r="15" spans="1:45" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="12"/>
+      <c r="B15" s="12"/>
+      <c r="C15" s="12"/>
+      <c r="D15" s="12"/>
+      <c r="E15" s="12"/>
+      <c r="F15" s="12"/>
       <c r="G15" s="3"/>
       <c r="H15" s="3"/>
       <c r="I15" s="2"/>
       <c r="J15" s="2"/>
-      <c r="K15" s="25"/>
+      <c r="K15" s="11"/>
       <c r="L15" s="2"/>
       <c r="M15" s="2"/>
       <c r="N15" s="2"/>
@@ -1594,9 +1657,15 @@
       <c r="AJ15" s="2"/>
       <c r="AK15" s="2"/>
       <c r="AL15" s="2"/>
-      <c r="AM15" s="48"/>
-    </row>
-    <row r="16" spans="1:39" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AM15" s="2"/>
+      <c r="AN15" s="2"/>
+      <c r="AO15" s="2"/>
+      <c r="AP15" s="2"/>
+      <c r="AQ15" s="2"/>
+      <c r="AR15" s="2"/>
+      <c r="AS15" s="2"/>
+    </row>
+    <row r="16" spans="1:45" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="1"/>
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
@@ -1607,7 +1676,7 @@
       <c r="H16" s="2"/>
       <c r="I16" s="2"/>
       <c r="J16" s="2"/>
-      <c r="K16" s="25"/>
+      <c r="K16" s="11"/>
       <c r="L16" s="2"/>
       <c r="M16" s="2"/>
       <c r="N16" s="2"/>
@@ -1635,9 +1704,15 @@
       <c r="AJ16" s="2"/>
       <c r="AK16" s="2"/>
       <c r="AL16" s="2"/>
-      <c r="AM16" s="48"/>
-    </row>
-    <row r="17" spans="1:39" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="AM16" s="2"/>
+      <c r="AN16" s="2"/>
+      <c r="AO16" s="2"/>
+      <c r="AP16" s="2"/>
+      <c r="AQ16" s="2"/>
+      <c r="AR16" s="2"/>
+      <c r="AS16" s="2"/>
+    </row>
+    <row r="17" spans="1:46" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
@@ -1648,7 +1723,7 @@
       <c r="H17" s="2"/>
       <c r="I17" s="2"/>
       <c r="J17" s="2"/>
-      <c r="K17" s="25"/>
+      <c r="K17" s="11"/>
       <c r="L17" s="2"/>
       <c r="M17" s="2"/>
       <c r="N17" s="2"/>
@@ -1676,9 +1751,15 @@
       <c r="AJ17" s="2"/>
       <c r="AK17" s="2"/>
       <c r="AL17" s="2"/>
-      <c r="AM17" s="48"/>
-    </row>
-    <row r="18" spans="1:39" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="AM17" s="2"/>
+      <c r="AN17" s="2"/>
+      <c r="AO17" s="2"/>
+      <c r="AP17" s="2"/>
+      <c r="AQ17" s="2"/>
+      <c r="AR17" s="2"/>
+      <c r="AS17" s="2"/>
+    </row>
+    <row r="18" spans="1:46" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
@@ -1689,22 +1770,22 @@
       <c r="H18" s="2"/>
       <c r="I18" s="2"/>
       <c r="J18" s="2"/>
-      <c r="K18" s="25"/>
-      <c r="L18" s="37"/>
-      <c r="M18" s="7" t="s">
+      <c r="K18" s="11"/>
+      <c r="L18" s="20"/>
+      <c r="M18" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="N18" s="8"/>
-      <c r="O18" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="P18" s="10"/>
-      <c r="Q18" s="10"/>
-      <c r="R18" s="10"/>
-      <c r="S18" s="10"/>
-      <c r="T18" s="10"/>
-      <c r="U18" s="10"/>
-      <c r="V18" s="11"/>
+      <c r="N18" s="30"/>
+      <c r="O18" s="31" t="s">
+        <v>58</v>
+      </c>
+      <c r="P18" s="31"/>
+      <c r="Q18" s="31"/>
+      <c r="R18" s="31"/>
+      <c r="S18" s="31"/>
+      <c r="T18" s="31"/>
+      <c r="U18" s="31"/>
+      <c r="V18" s="32"/>
       <c r="W18" s="2"/>
       <c r="X18" s="2"/>
       <c r="Y18" s="2"/>
@@ -1721,9 +1802,15 @@
       <c r="AJ18" s="2"/>
       <c r="AK18" s="2"/>
       <c r="AL18" s="2"/>
-      <c r="AM18" s="48"/>
-    </row>
-    <row r="19" spans="1:39" ht="18.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="AM18" s="2"/>
+      <c r="AN18" s="2"/>
+      <c r="AO18" s="2"/>
+      <c r="AP18" s="2"/>
+      <c r="AQ18" s="2"/>
+      <c r="AR18" s="2"/>
+      <c r="AS18" s="2"/>
+    </row>
+    <row r="19" spans="1:46" ht="18.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A19" s="1"/>
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
@@ -1736,18 +1823,18 @@
       <c r="J19" s="2"/>
       <c r="K19" s="2"/>
       <c r="L19" s="2"/>
-      <c r="M19" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="N19" s="15"/>
-      <c r="O19" s="15"/>
-      <c r="P19" s="15"/>
-      <c r="Q19" s="15"/>
-      <c r="R19" s="15"/>
-      <c r="S19" s="15"/>
-      <c r="T19" s="15"/>
-      <c r="U19" s="15"/>
-      <c r="V19" s="16"/>
+      <c r="M19" s="33" t="s">
+        <v>59</v>
+      </c>
+      <c r="N19" s="34"/>
+      <c r="O19" s="34"/>
+      <c r="P19" s="34"/>
+      <c r="Q19" s="34"/>
+      <c r="R19" s="34"/>
+      <c r="S19" s="34"/>
+      <c r="T19" s="34"/>
+      <c r="U19" s="34"/>
+      <c r="V19" s="35"/>
       <c r="W19" s="2"/>
       <c r="X19" s="2"/>
       <c r="Y19" s="2"/>
@@ -1764,9 +1851,15 @@
       <c r="AJ19" s="2"/>
       <c r="AK19" s="2"/>
       <c r="AL19" s="2"/>
-      <c r="AM19" s="48"/>
-    </row>
-    <row r="20" spans="1:39" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="AM19" s="2"/>
+      <c r="AN19" s="2"/>
+      <c r="AO19" s="2"/>
+      <c r="AP19" s="2"/>
+      <c r="AQ19" s="2"/>
+      <c r="AR19" s="2"/>
+      <c r="AS19" s="2"/>
+    </row>
+    <row r="20" spans="1:46" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
@@ -1779,18 +1872,18 @@
       <c r="J20" s="2"/>
       <c r="K20" s="2"/>
       <c r="L20" s="2"/>
-      <c r="M20" s="22" t="s">
-        <v>15</v>
-      </c>
-      <c r="N20" s="23"/>
-      <c r="O20" s="23"/>
-      <c r="P20" s="23"/>
-      <c r="Q20" s="23"/>
-      <c r="R20" s="23"/>
-      <c r="S20" s="23"/>
-      <c r="T20" s="23"/>
-      <c r="U20" s="23"/>
-      <c r="V20" s="24"/>
+      <c r="M20" s="36" t="s">
+        <v>60</v>
+      </c>
+      <c r="N20" s="37"/>
+      <c r="O20" s="37"/>
+      <c r="P20" s="37"/>
+      <c r="Q20" s="37"/>
+      <c r="R20" s="37"/>
+      <c r="S20" s="37"/>
+      <c r="T20" s="37"/>
+      <c r="U20" s="37"/>
+      <c r="V20" s="38"/>
       <c r="W20" s="2"/>
       <c r="X20" s="2"/>
       <c r="Y20" s="2"/>
@@ -1807,9 +1900,15 @@
       <c r="AJ20" s="2"/>
       <c r="AK20" s="2"/>
       <c r="AL20" s="2"/>
-      <c r="AM20" s="48"/>
-    </row>
-    <row r="21" spans="1:39" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AM20" s="2"/>
+      <c r="AN20" s="2"/>
+      <c r="AO20" s="2"/>
+      <c r="AP20" s="2"/>
+      <c r="AQ20" s="2"/>
+      <c r="AR20" s="2"/>
+      <c r="AS20" s="2"/>
+    </row>
+    <row r="21" spans="1:46" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="1"/>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
@@ -1848,9 +1947,15 @@
       <c r="AJ21" s="2"/>
       <c r="AK21" s="2"/>
       <c r="AL21" s="2"/>
-      <c r="AM21" s="48"/>
-    </row>
-    <row r="22" spans="1:39" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AM21" s="2"/>
+      <c r="AN21" s="2"/>
+      <c r="AO21" s="2"/>
+      <c r="AP21" s="2"/>
+      <c r="AQ21" s="2"/>
+      <c r="AR21" s="2"/>
+      <c r="AS21" s="2"/>
+    </row>
+    <row r="22" spans="1:46" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="1"/>
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
@@ -1889,9 +1994,15 @@
       <c r="AJ22" s="2"/>
       <c r="AK22" s="2"/>
       <c r="AL22" s="2"/>
-      <c r="AM22" s="48"/>
-    </row>
-    <row r="23" spans="1:39" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AM22" s="2"/>
+      <c r="AN22" s="2"/>
+      <c r="AO22" s="2"/>
+      <c r="AP22" s="2"/>
+      <c r="AQ22" s="2"/>
+      <c r="AR22" s="2"/>
+      <c r="AS22" s="2"/>
+    </row>
+    <row r="23" spans="1:46" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="1"/>
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
@@ -1930,9 +2041,15 @@
       <c r="AJ23" s="2"/>
       <c r="AK23" s="2"/>
       <c r="AL23" s="2"/>
-      <c r="AM23" s="48"/>
-    </row>
-    <row r="24" spans="1:39" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="AM23" s="2"/>
+      <c r="AN23" s="2"/>
+      <c r="AO23" s="2"/>
+      <c r="AP23" s="2"/>
+      <c r="AQ23" s="2"/>
+      <c r="AR23" s="2"/>
+      <c r="AS23" s="2"/>
+    </row>
+    <row r="24" spans="1:46" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
@@ -1971,28 +2088,34 @@
       <c r="AJ24" s="2"/>
       <c r="AK24" s="2"/>
       <c r="AL24" s="2"/>
-      <c r="AM24" s="48"/>
-    </row>
-    <row r="25" spans="1:39" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="38" t="s">
+      <c r="AM24" s="2"/>
+      <c r="AN24" s="2"/>
+      <c r="AO24" s="2"/>
+      <c r="AP24" s="2"/>
+      <c r="AQ24" s="2"/>
+      <c r="AR24" s="2"/>
+      <c r="AS24" s="2"/>
+    </row>
+    <row r="25" spans="1:46" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="39" t="s">
         <v>0</v>
       </c>
-      <c r="B25" s="39"/>
-      <c r="C25" s="39"/>
-      <c r="D25" s="39"/>
-      <c r="E25" s="39"/>
-      <c r="F25" s="39"/>
-      <c r="G25" s="39"/>
-      <c r="H25" s="39"/>
-      <c r="I25" s="39"/>
-      <c r="J25" s="39"/>
-      <c r="K25" s="39"/>
-      <c r="L25" s="39"/>
-      <c r="M25" s="39"/>
-      <c r="N25" s="39"/>
-      <c r="O25" s="39"/>
-      <c r="P25" s="39"/>
-      <c r="Q25" s="40"/>
+      <c r="B25" s="40"/>
+      <c r="C25" s="40"/>
+      <c r="D25" s="40"/>
+      <c r="E25" s="40"/>
+      <c r="F25" s="40"/>
+      <c r="G25" s="40"/>
+      <c r="H25" s="40"/>
+      <c r="I25" s="40"/>
+      <c r="J25" s="40"/>
+      <c r="K25" s="40"/>
+      <c r="L25" s="40"/>
+      <c r="M25" s="40"/>
+      <c r="N25" s="40"/>
+      <c r="O25" s="40"/>
+      <c r="P25" s="40"/>
+      <c r="Q25" s="41"/>
       <c r="R25" s="2"/>
       <c r="S25" s="2"/>
       <c r="T25" s="2"/>
@@ -2014,57 +2137,95 @@
       <c r="AJ25" s="2"/>
       <c r="AK25" s="2"/>
       <c r="AL25" s="2"/>
-      <c r="AM25" s="48"/>
-    </row>
-    <row r="26" spans="1:39" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="41"/>
-      <c r="B26" s="42"/>
-      <c r="C26" s="42"/>
-      <c r="D26" s="42"/>
-      <c r="E26" s="42"/>
-      <c r="F26" s="42"/>
-      <c r="G26" s="42"/>
-      <c r="H26" s="42"/>
-      <c r="I26" s="42"/>
-      <c r="J26" s="42"/>
-      <c r="K26" s="42"/>
-      <c r="L26" s="42"/>
-      <c r="M26" s="42"/>
-      <c r="N26" s="42"/>
-      <c r="O26" s="42"/>
-      <c r="P26" s="42"/>
-      <c r="Q26" s="43"/>
-      <c r="R26" s="44"/>
-      <c r="S26" s="44"/>
-      <c r="T26" s="44"/>
-      <c r="U26" s="44"/>
-      <c r="V26" s="44"/>
-      <c r="W26" s="44"/>
-      <c r="X26" s="44"/>
-      <c r="Y26" s="44"/>
-      <c r="Z26" s="44"/>
-      <c r="AA26" s="44"/>
-      <c r="AB26" s="44"/>
-      <c r="AC26" s="44"/>
-      <c r="AD26" s="44"/>
-      <c r="AE26" s="44"/>
-      <c r="AF26" s="44"/>
-      <c r="AG26" s="44"/>
-      <c r="AH26" s="44"/>
-      <c r="AI26" s="44"/>
-      <c r="AJ26" s="44"/>
-      <c r="AK26" s="44"/>
-      <c r="AL26" s="44"/>
-      <c r="AM26" s="52"/>
+      <c r="AM25" s="2"/>
+      <c r="AN25" s="2"/>
+      <c r="AO25" s="2"/>
+      <c r="AP25" s="2"/>
+      <c r="AQ25" s="2"/>
+      <c r="AR25" s="2"/>
+      <c r="AS25" s="2"/>
+    </row>
+    <row r="26" spans="1:46" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="42"/>
+      <c r="B26" s="43"/>
+      <c r="C26" s="43"/>
+      <c r="D26" s="43"/>
+      <c r="E26" s="43"/>
+      <c r="F26" s="43"/>
+      <c r="G26" s="43"/>
+      <c r="H26" s="43"/>
+      <c r="I26" s="43"/>
+      <c r="J26" s="43"/>
+      <c r="K26" s="43"/>
+      <c r="L26" s="43"/>
+      <c r="M26" s="43"/>
+      <c r="N26" s="43"/>
+      <c r="O26" s="43"/>
+      <c r="P26" s="43"/>
+      <c r="Q26" s="44"/>
+      <c r="R26" s="21"/>
+      <c r="S26" s="21"/>
+      <c r="T26" s="21"/>
+      <c r="U26" s="21"/>
+      <c r="V26" s="21"/>
+      <c r="W26" s="21"/>
+      <c r="X26" s="21"/>
+      <c r="Y26" s="21"/>
+      <c r="Z26" s="21"/>
+      <c r="AA26" s="21"/>
+      <c r="AB26" s="21"/>
+      <c r="AC26" s="21"/>
+      <c r="AD26" s="21"/>
+      <c r="AE26" s="21"/>
+      <c r="AF26" s="21"/>
+      <c r="AG26" s="21"/>
+      <c r="AH26" s="21"/>
+      <c r="AI26" s="27"/>
+      <c r="AJ26" s="21"/>
+      <c r="AK26" s="21"/>
+      <c r="AL26" s="21"/>
+      <c r="AM26" s="21"/>
+      <c r="AN26" s="52"/>
+      <c r="AO26" s="52"/>
+      <c r="AP26" s="52"/>
+      <c r="AQ26" s="52"/>
+      <c r="AR26" s="52"/>
+      <c r="AS26" s="52"/>
+      <c r="AT26" s="52"/>
+    </row>
+    <row r="27" spans="1:46" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="R27" s="6"/>
+      <c r="S27" s="6"/>
+      <c r="T27" s="6"/>
+      <c r="U27" s="6"/>
+      <c r="V27" s="6"/>
+      <c r="W27" s="6"/>
+      <c r="X27" s="6"/>
+      <c r="Y27" s="6"/>
+      <c r="Z27" s="6"/>
+      <c r="AA27" s="6"/>
+      <c r="AB27" s="6"/>
+      <c r="AC27" s="6"/>
+      <c r="AD27" s="6"/>
+      <c r="AE27" s="6"/>
+      <c r="AF27" s="6"/>
+      <c r="AG27" s="6"/>
+      <c r="AH27" s="6"/>
+      <c r="AI27" s="6"/>
+      <c r="AJ27" s="6"/>
+      <c r="AK27" s="6"/>
+      <c r="AL27" s="6"/>
+      <c r="AM27" s="6"/>
+      <c r="AN27" s="6"/>
+      <c r="AO27" s="6"/>
+      <c r="AP27" s="6"/>
+      <c r="AQ27" s="6"/>
+      <c r="AR27" s="6"/>
+      <c r="AS27" s="6"/>
+      <c r="AT27" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="M20:V20"/>
-    <mergeCell ref="M11:V11"/>
-    <mergeCell ref="M12:V12"/>
-    <mergeCell ref="M18:N18"/>
-    <mergeCell ref="O18:V18"/>
-    <mergeCell ref="M19:V19"/>
     <mergeCell ref="M2:N2"/>
     <mergeCell ref="O2:V2"/>
     <mergeCell ref="M3:V3"/>
@@ -2076,8 +2237,14 @@
     <mergeCell ref="A11:J11"/>
     <mergeCell ref="A12:J12"/>
     <mergeCell ref="A25:Q26"/>
+    <mergeCell ref="M20:V20"/>
+    <mergeCell ref="M11:V11"/>
+    <mergeCell ref="M12:V12"/>
+    <mergeCell ref="M18:N18"/>
+    <mergeCell ref="O18:V18"/>
+    <mergeCell ref="M19:V19"/>
   </mergeCells>
-  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.86614173228346458" right="0.86614173228346458" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
@@ -2087,10 +2254,10 @@
   <sheetPr>
     <tabColor theme="8" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A1:AM26"/>
+  <dimension ref="A1:AT26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="V23" sqref="V23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="3.5703125" defaultRowHeight="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2137,35 +2304,35 @@
       <c r="AJ1" s="4"/>
       <c r="AK1" s="4"/>
       <c r="AL1" s="4"/>
-      <c r="AM1" s="46"/>
+      <c r="AM1" s="4"/>
     </row>
     <row r="2" spans="1:39" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="29" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="8"/>
-      <c r="C2" s="10" t="s">
+      <c r="B2" s="30"/>
+      <c r="C2" s="31" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="10"/>
-      <c r="E2" s="10"/>
-      <c r="F2" s="10"/>
-      <c r="G2" s="10"/>
-      <c r="H2" s="10"/>
-      <c r="I2" s="10"/>
-      <c r="J2" s="11"/>
+      <c r="D2" s="31"/>
+      <c r="E2" s="31"/>
+      <c r="F2" s="31"/>
+      <c r="G2" s="31"/>
+      <c r="H2" s="31"/>
+      <c r="I2" s="31"/>
+      <c r="J2" s="32"/>
       <c r="K2" s="2"/>
       <c r="L2" s="3"/>
-      <c r="M2" s="53"/>
-      <c r="N2" s="53"/>
-      <c r="O2" s="29"/>
-      <c r="P2" s="29"/>
-      <c r="Q2" s="29"/>
-      <c r="R2" s="29"/>
-      <c r="S2" s="29"/>
-      <c r="T2" s="29"/>
-      <c r="U2" s="29"/>
-      <c r="V2" s="29"/>
+      <c r="M2" s="28"/>
+      <c r="N2" s="28"/>
+      <c r="O2" s="12"/>
+      <c r="P2" s="12"/>
+      <c r="Q2" s="12"/>
+      <c r="R2" s="12"/>
+      <c r="S2" s="12"/>
+      <c r="T2" s="12"/>
+      <c r="U2" s="12"/>
+      <c r="V2" s="12"/>
       <c r="W2" s="3"/>
       <c r="X2" s="2"/>
       <c r="Y2" s="2"/>
@@ -2182,33 +2349,33 @@
       <c r="AJ2" s="2"/>
       <c r="AK2" s="2"/>
       <c r="AL2" s="2"/>
-      <c r="AM2" s="48"/>
+      <c r="AM2" s="2"/>
     </row>
     <row r="3" spans="1:39" ht="18.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="14" t="s">
+      <c r="A3" s="33" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="15"/>
-      <c r="C3" s="15"/>
-      <c r="D3" s="15"/>
-      <c r="E3" s="15"/>
-      <c r="F3" s="15"/>
-      <c r="G3" s="15"/>
-      <c r="H3" s="15"/>
-      <c r="I3" s="15"/>
-      <c r="J3" s="16"/>
-      <c r="K3" s="51"/>
+      <c r="B3" s="34"/>
+      <c r="C3" s="34"/>
+      <c r="D3" s="34"/>
+      <c r="E3" s="34"/>
+      <c r="F3" s="34"/>
+      <c r="G3" s="34"/>
+      <c r="H3" s="34"/>
+      <c r="I3" s="34"/>
+      <c r="J3" s="35"/>
+      <c r="K3" s="26"/>
       <c r="L3" s="3"/>
-      <c r="M3" s="29"/>
-      <c r="N3" s="29"/>
-      <c r="O3" s="29"/>
-      <c r="P3" s="29"/>
-      <c r="Q3" s="29"/>
-      <c r="R3" s="29"/>
-      <c r="S3" s="29"/>
-      <c r="T3" s="29"/>
-      <c r="U3" s="29"/>
-      <c r="V3" s="29"/>
+      <c r="M3" s="12"/>
+      <c r="N3" s="12"/>
+      <c r="O3" s="12"/>
+      <c r="P3" s="12"/>
+      <c r="Q3" s="12"/>
+      <c r="R3" s="12"/>
+      <c r="S3" s="12"/>
+      <c r="T3" s="12"/>
+      <c r="U3" s="12"/>
+      <c r="V3" s="12"/>
       <c r="W3" s="3"/>
       <c r="X3" s="2"/>
       <c r="Y3" s="2"/>
@@ -2225,31 +2392,31 @@
       <c r="AJ3" s="2"/>
       <c r="AK3" s="2"/>
       <c r="AL3" s="2"/>
-      <c r="AM3" s="48"/>
+      <c r="AM3" s="2"/>
     </row>
     <row r="4" spans="1:39" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="22"/>
-      <c r="B4" s="23"/>
-      <c r="C4" s="23"/>
-      <c r="D4" s="23"/>
-      <c r="E4" s="23"/>
-      <c r="F4" s="23"/>
-      <c r="G4" s="23"/>
-      <c r="H4" s="23"/>
-      <c r="I4" s="23"/>
-      <c r="J4" s="24"/>
+      <c r="A4" s="36"/>
+      <c r="B4" s="37"/>
+      <c r="C4" s="37"/>
+      <c r="D4" s="37"/>
+      <c r="E4" s="37"/>
+      <c r="F4" s="37"/>
+      <c r="G4" s="37"/>
+      <c r="H4" s="37"/>
+      <c r="I4" s="37"/>
+      <c r="J4" s="38"/>
       <c r="K4" s="2"/>
       <c r="L4" s="3"/>
-      <c r="M4" s="29"/>
-      <c r="N4" s="29"/>
-      <c r="O4" s="29"/>
-      <c r="P4" s="29"/>
-      <c r="Q4" s="29"/>
-      <c r="R4" s="29"/>
-      <c r="S4" s="29"/>
-      <c r="T4" s="29"/>
-      <c r="U4" s="29"/>
-      <c r="V4" s="29"/>
+      <c r="M4" s="12"/>
+      <c r="N4" s="12"/>
+      <c r="O4" s="12"/>
+      <c r="P4" s="12"/>
+      <c r="Q4" s="12"/>
+      <c r="R4" s="12"/>
+      <c r="S4" s="12"/>
+      <c r="T4" s="12"/>
+      <c r="U4" s="12"/>
+      <c r="V4" s="12"/>
       <c r="W4" s="3"/>
       <c r="X4" s="2"/>
       <c r="Y4" s="2"/>
@@ -2266,18 +2433,18 @@
       <c r="AJ4" s="2"/>
       <c r="AK4" s="2"/>
       <c r="AL4" s="2"/>
-      <c r="AM4" s="48"/>
+      <c r="AM4" s="2"/>
     </row>
     <row r="5" spans="1:39" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="29"/>
-      <c r="B5" s="29"/>
-      <c r="C5" s="29"/>
-      <c r="D5" s="29"/>
-      <c r="E5" s="29"/>
-      <c r="F5" s="29"/>
-      <c r="G5" s="29"/>
-      <c r="H5" s="29"/>
-      <c r="I5" s="29"/>
+      <c r="A5" s="12"/>
+      <c r="B5" s="12"/>
+      <c r="C5" s="12"/>
+      <c r="D5" s="12"/>
+      <c r="E5" s="12"/>
+      <c r="F5" s="12"/>
+      <c r="G5" s="12"/>
+      <c r="H5" s="12"/>
+      <c r="I5" s="12"/>
       <c r="J5" s="2"/>
       <c r="K5" s="2"/>
       <c r="L5" s="3"/>
@@ -2307,7 +2474,7 @@
       <c r="AJ5" s="2"/>
       <c r="AK5" s="2"/>
       <c r="AL5" s="2"/>
-      <c r="AM5" s="48"/>
+      <c r="AM5" s="2"/>
     </row>
     <row r="6" spans="1:39" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
@@ -2348,7 +2515,7 @@
       <c r="AJ6" s="2"/>
       <c r="AK6" s="2"/>
       <c r="AL6" s="2"/>
-      <c r="AM6" s="48"/>
+      <c r="AM6" s="2"/>
     </row>
     <row r="7" spans="1:39" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
@@ -2389,7 +2556,7 @@
       <c r="AJ7" s="2"/>
       <c r="AK7" s="2"/>
       <c r="AL7" s="2"/>
-      <c r="AM7" s="48"/>
+      <c r="AM7" s="2"/>
     </row>
     <row r="8" spans="1:39" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
@@ -2430,7 +2597,7 @@
       <c r="AJ8" s="2"/>
       <c r="AK8" s="2"/>
       <c r="AL8" s="2"/>
-      <c r="AM8" s="48"/>
+      <c r="AM8" s="2"/>
     </row>
     <row r="9" spans="1:39" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="L9" s="3"/>
@@ -2460,20 +2627,20 @@
       <c r="AJ9" s="2"/>
       <c r="AK9" s="2"/>
       <c r="AL9" s="2"/>
-      <c r="AM9" s="48"/>
+      <c r="AM9" s="2"/>
     </row>
     <row r="10" spans="1:39" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="L10" s="3"/>
-      <c r="M10" s="53"/>
-      <c r="N10" s="53"/>
-      <c r="O10" s="29"/>
-      <c r="P10" s="29"/>
-      <c r="Q10" s="29"/>
-      <c r="R10" s="29"/>
-      <c r="S10" s="29"/>
-      <c r="T10" s="29"/>
-      <c r="U10" s="29"/>
-      <c r="V10" s="29"/>
+      <c r="M10" s="28"/>
+      <c r="N10" s="28"/>
+      <c r="O10" s="12"/>
+      <c r="P10" s="12"/>
+      <c r="Q10" s="12"/>
+      <c r="R10" s="12"/>
+      <c r="S10" s="12"/>
+      <c r="T10" s="12"/>
+      <c r="U10" s="12"/>
+      <c r="V10" s="12"/>
       <c r="W10" s="3"/>
       <c r="X10" s="2"/>
       <c r="Y10" s="2"/>
@@ -2490,20 +2657,20 @@
       <c r="AJ10" s="2"/>
       <c r="AK10" s="2"/>
       <c r="AL10" s="2"/>
-      <c r="AM10" s="48"/>
+      <c r="AM10" s="2"/>
     </row>
     <row r="11" spans="1:39" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="L11" s="3"/>
-      <c r="M11" s="29"/>
-      <c r="N11" s="29"/>
-      <c r="O11" s="29"/>
-      <c r="P11" s="29"/>
-      <c r="Q11" s="29"/>
-      <c r="R11" s="29"/>
-      <c r="S11" s="29"/>
-      <c r="T11" s="29"/>
-      <c r="U11" s="29"/>
-      <c r="V11" s="29"/>
+      <c r="M11" s="12"/>
+      <c r="N11" s="12"/>
+      <c r="O11" s="12"/>
+      <c r="P11" s="12"/>
+      <c r="Q11" s="12"/>
+      <c r="R11" s="12"/>
+      <c r="S11" s="12"/>
+      <c r="T11" s="12"/>
+      <c r="U11" s="12"/>
+      <c r="V11" s="12"/>
       <c r="W11" s="3"/>
       <c r="X11" s="2"/>
       <c r="Y11" s="2"/>
@@ -2520,20 +2687,20 @@
       <c r="AJ11" s="2"/>
       <c r="AK11" s="2"/>
       <c r="AL11" s="2"/>
-      <c r="AM11" s="48"/>
+      <c r="AM11" s="2"/>
     </row>
     <row r="12" spans="1:39" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="L12" s="3"/>
-      <c r="M12" s="29"/>
-      <c r="N12" s="29"/>
-      <c r="O12" s="29"/>
-      <c r="P12" s="29"/>
-      <c r="Q12" s="29"/>
-      <c r="R12" s="29"/>
-      <c r="S12" s="29"/>
-      <c r="T12" s="29"/>
-      <c r="U12" s="29"/>
-      <c r="V12" s="29"/>
+      <c r="M12" s="12"/>
+      <c r="N12" s="12"/>
+      <c r="O12" s="12"/>
+      <c r="P12" s="12"/>
+      <c r="Q12" s="12"/>
+      <c r="R12" s="12"/>
+      <c r="S12" s="12"/>
+      <c r="T12" s="12"/>
+      <c r="U12" s="12"/>
+      <c r="V12" s="12"/>
       <c r="W12" s="3"/>
       <c r="X12" s="2"/>
       <c r="Y12" s="2"/>
@@ -2550,7 +2717,7 @@
       <c r="AJ12" s="2"/>
       <c r="AK12" s="2"/>
       <c r="AL12" s="2"/>
-      <c r="AM12" s="48"/>
+      <c r="AM12" s="2"/>
     </row>
     <row r="13" spans="1:39" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="L13" s="3"/>
@@ -2580,18 +2747,18 @@
       <c r="AJ13" s="2"/>
       <c r="AK13" s="2"/>
       <c r="AL13" s="2"/>
-      <c r="AM13" s="48"/>
+      <c r="AM13" s="2"/>
     </row>
     <row r="14" spans="1:39" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="29"/>
-      <c r="B14" s="29"/>
-      <c r="C14" s="29"/>
-      <c r="D14" s="29"/>
-      <c r="E14" s="29"/>
-      <c r="F14" s="29"/>
-      <c r="G14" s="29"/>
-      <c r="H14" s="29"/>
-      <c r="I14" s="29"/>
+      <c r="A14" s="12"/>
+      <c r="B14" s="12"/>
+      <c r="C14" s="12"/>
+      <c r="D14" s="12"/>
+      <c r="E14" s="12"/>
+      <c r="F14" s="12"/>
+      <c r="G14" s="12"/>
+      <c r="H14" s="12"/>
+      <c r="I14" s="12"/>
       <c r="J14" s="2"/>
       <c r="K14" s="2"/>
       <c r="L14" s="3"/>
@@ -2621,15 +2788,15 @@
       <c r="AJ14" s="2"/>
       <c r="AK14" s="2"/>
       <c r="AL14" s="2"/>
-      <c r="AM14" s="48"/>
+      <c r="AM14" s="2"/>
     </row>
     <row r="15" spans="1:39" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="29"/>
-      <c r="B15" s="29"/>
-      <c r="C15" s="29"/>
-      <c r="D15" s="29"/>
-      <c r="E15" s="29"/>
-      <c r="F15" s="29"/>
+      <c r="A15" s="12"/>
+      <c r="B15" s="12"/>
+      <c r="C15" s="12"/>
+      <c r="D15" s="12"/>
+      <c r="E15" s="12"/>
+      <c r="F15" s="12"/>
       <c r="G15" s="3"/>
       <c r="H15" s="3"/>
       <c r="I15" s="2"/>
@@ -2662,7 +2829,7 @@
       <c r="AJ15" s="2"/>
       <c r="AK15" s="2"/>
       <c r="AL15" s="2"/>
-      <c r="AM15" s="48"/>
+      <c r="AM15" s="2"/>
     </row>
     <row r="16" spans="1:39" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
@@ -2703,9 +2870,9 @@
       <c r="AJ16" s="2"/>
       <c r="AK16" s="2"/>
       <c r="AL16" s="2"/>
-      <c r="AM16" s="48"/>
-    </row>
-    <row r="17" spans="1:39" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AM16" s="2"/>
+    </row>
+    <row r="17" spans="1:46" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
@@ -2744,9 +2911,9 @@
       <c r="AJ17" s="2"/>
       <c r="AK17" s="2"/>
       <c r="AL17" s="2"/>
-      <c r="AM17" s="48"/>
-    </row>
-    <row r="18" spans="1:39" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AM17" s="2"/>
+    </row>
+    <row r="18" spans="1:46" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
@@ -2759,16 +2926,16 @@
       <c r="J18" s="2"/>
       <c r="K18" s="2"/>
       <c r="L18" s="3"/>
-      <c r="M18" s="53"/>
-      <c r="N18" s="53"/>
-      <c r="O18" s="29"/>
-      <c r="P18" s="29"/>
-      <c r="Q18" s="29"/>
-      <c r="R18" s="29"/>
-      <c r="S18" s="29"/>
-      <c r="T18" s="29"/>
-      <c r="U18" s="29"/>
-      <c r="V18" s="29"/>
+      <c r="M18" s="28"/>
+      <c r="N18" s="28"/>
+      <c r="O18" s="12"/>
+      <c r="P18" s="12"/>
+      <c r="Q18" s="12"/>
+      <c r="R18" s="12"/>
+      <c r="S18" s="12"/>
+      <c r="T18" s="12"/>
+      <c r="U18" s="12"/>
+      <c r="V18" s="12"/>
       <c r="W18" s="3"/>
       <c r="X18" s="2"/>
       <c r="Y18" s="2"/>
@@ -2785,9 +2952,9 @@
       <c r="AJ18" s="2"/>
       <c r="AK18" s="2"/>
       <c r="AL18" s="2"/>
-      <c r="AM18" s="48"/>
-    </row>
-    <row r="19" spans="1:39" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AM18" s="2"/>
+    </row>
+    <row r="19" spans="1:46" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
@@ -2800,16 +2967,16 @@
       <c r="J19" s="2"/>
       <c r="K19" s="2"/>
       <c r="L19" s="3"/>
-      <c r="M19" s="29"/>
-      <c r="N19" s="29"/>
-      <c r="O19" s="29"/>
-      <c r="P19" s="29"/>
-      <c r="Q19" s="29"/>
-      <c r="R19" s="29"/>
-      <c r="S19" s="29"/>
-      <c r="T19" s="29"/>
-      <c r="U19" s="29"/>
-      <c r="V19" s="29"/>
+      <c r="M19" s="12"/>
+      <c r="N19" s="12"/>
+      <c r="O19" s="12"/>
+      <c r="P19" s="12"/>
+      <c r="Q19" s="12"/>
+      <c r="R19" s="12"/>
+      <c r="S19" s="12"/>
+      <c r="T19" s="12"/>
+      <c r="U19" s="12"/>
+      <c r="V19" s="12"/>
       <c r="W19" s="3"/>
       <c r="X19" s="2"/>
       <c r="Y19" s="2"/>
@@ -2826,9 +2993,9 @@
       <c r="AJ19" s="2"/>
       <c r="AK19" s="2"/>
       <c r="AL19" s="2"/>
-      <c r="AM19" s="48"/>
-    </row>
-    <row r="20" spans="1:39" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AM19" s="2"/>
+    </row>
+    <row r="20" spans="1:46" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
@@ -2841,16 +3008,16 @@
       <c r="J20" s="2"/>
       <c r="K20" s="2"/>
       <c r="L20" s="3"/>
-      <c r="M20" s="29"/>
-      <c r="N20" s="29"/>
-      <c r="O20" s="29"/>
-      <c r="P20" s="29"/>
-      <c r="Q20" s="29"/>
-      <c r="R20" s="29"/>
-      <c r="S20" s="29"/>
-      <c r="T20" s="29"/>
-      <c r="U20" s="29"/>
-      <c r="V20" s="29"/>
+      <c r="M20" s="12"/>
+      <c r="N20" s="12"/>
+      <c r="O20" s="12"/>
+      <c r="P20" s="12"/>
+      <c r="Q20" s="12"/>
+      <c r="R20" s="12"/>
+      <c r="S20" s="12"/>
+      <c r="T20" s="12"/>
+      <c r="U20" s="12"/>
+      <c r="V20" s="12"/>
       <c r="W20" s="3"/>
       <c r="X20" s="2"/>
       <c r="Y20" s="2"/>
@@ -2867,9 +3034,9 @@
       <c r="AJ20" s="2"/>
       <c r="AK20" s="2"/>
       <c r="AL20" s="2"/>
-      <c r="AM20" s="48"/>
-    </row>
-    <row r="21" spans="1:39" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AM20" s="2"/>
+    </row>
+    <row r="21" spans="1:46" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
@@ -2908,9 +3075,9 @@
       <c r="AJ21" s="2"/>
       <c r="AK21" s="2"/>
       <c r="AL21" s="2"/>
-      <c r="AM21" s="48"/>
-    </row>
-    <row r="22" spans="1:39" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AM21" s="2"/>
+    </row>
+    <row r="22" spans="1:46" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
@@ -2949,9 +3116,9 @@
       <c r="AJ22" s="2"/>
       <c r="AK22" s="2"/>
       <c r="AL22" s="2"/>
-      <c r="AM22" s="48"/>
-    </row>
-    <row r="23" spans="1:39" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AM22" s="2"/>
+    </row>
+    <row r="23" spans="1:46" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
@@ -2990,9 +3157,9 @@
       <c r="AJ23" s="2"/>
       <c r="AK23" s="2"/>
       <c r="AL23" s="2"/>
-      <c r="AM23" s="48"/>
-    </row>
-    <row r="24" spans="1:39" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AM23" s="2"/>
+    </row>
+    <row r="24" spans="1:46" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="1"/>
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
@@ -3031,28 +3198,28 @@
       <c r="AJ24" s="2"/>
       <c r="AK24" s="2"/>
       <c r="AL24" s="2"/>
-      <c r="AM24" s="48"/>
-    </row>
-    <row r="25" spans="1:39" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="38" t="s">
-        <v>18</v>
-      </c>
-      <c r="B25" s="39"/>
-      <c r="C25" s="39"/>
-      <c r="D25" s="39"/>
-      <c r="E25" s="39"/>
-      <c r="F25" s="39"/>
-      <c r="G25" s="39"/>
-      <c r="H25" s="39"/>
-      <c r="I25" s="39"/>
-      <c r="J25" s="39"/>
-      <c r="K25" s="39"/>
-      <c r="L25" s="39"/>
-      <c r="M25" s="39"/>
-      <c r="N25" s="39"/>
-      <c r="O25" s="39"/>
-      <c r="P25" s="39"/>
-      <c r="Q25" s="40"/>
+      <c r="AM24" s="2"/>
+    </row>
+    <row r="25" spans="1:46" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="39" t="s">
+        <v>15</v>
+      </c>
+      <c r="B25" s="40"/>
+      <c r="C25" s="40"/>
+      <c r="D25" s="40"/>
+      <c r="E25" s="40"/>
+      <c r="F25" s="40"/>
+      <c r="G25" s="40"/>
+      <c r="H25" s="40"/>
+      <c r="I25" s="40"/>
+      <c r="J25" s="40"/>
+      <c r="K25" s="40"/>
+      <c r="L25" s="40"/>
+      <c r="M25" s="40"/>
+      <c r="N25" s="40"/>
+      <c r="O25" s="40"/>
+      <c r="P25" s="40"/>
+      <c r="Q25" s="41"/>
       <c r="R25" s="2"/>
       <c r="S25" s="2"/>
       <c r="T25" s="2"/>
@@ -3074,48 +3241,55 @@
       <c r="AJ25" s="2"/>
       <c r="AK25" s="2"/>
       <c r="AL25" s="2"/>
-      <c r="AM25" s="48"/>
-    </row>
-    <row r="26" spans="1:39" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="41"/>
-      <c r="B26" s="42"/>
-      <c r="C26" s="42"/>
-      <c r="D26" s="42"/>
-      <c r="E26" s="42"/>
-      <c r="F26" s="42"/>
-      <c r="G26" s="42"/>
-      <c r="H26" s="42"/>
-      <c r="I26" s="42"/>
-      <c r="J26" s="42"/>
-      <c r="K26" s="42"/>
-      <c r="L26" s="42"/>
-      <c r="M26" s="42"/>
-      <c r="N26" s="42"/>
-      <c r="O26" s="42"/>
-      <c r="P26" s="42"/>
-      <c r="Q26" s="43"/>
-      <c r="R26" s="44"/>
-      <c r="S26" s="44"/>
-      <c r="T26" s="44"/>
-      <c r="U26" s="44"/>
-      <c r="V26" s="44"/>
-      <c r="W26" s="44"/>
-      <c r="X26" s="44"/>
-      <c r="Y26" s="44"/>
-      <c r="Z26" s="44"/>
-      <c r="AA26" s="44"/>
-      <c r="AB26" s="44"/>
-      <c r="AC26" s="44"/>
-      <c r="AD26" s="44"/>
-      <c r="AE26" s="44"/>
-      <c r="AF26" s="44"/>
-      <c r="AG26" s="44"/>
-      <c r="AH26" s="44"/>
-      <c r="AI26" s="44"/>
-      <c r="AJ26" s="44"/>
-      <c r="AK26" s="44"/>
-      <c r="AL26" s="44"/>
-      <c r="AM26" s="52"/>
+      <c r="AM25" s="2"/>
+    </row>
+    <row r="26" spans="1:46" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="42"/>
+      <c r="B26" s="43"/>
+      <c r="C26" s="43"/>
+      <c r="D26" s="43"/>
+      <c r="E26" s="43"/>
+      <c r="F26" s="43"/>
+      <c r="G26" s="43"/>
+      <c r="H26" s="43"/>
+      <c r="I26" s="43"/>
+      <c r="J26" s="43"/>
+      <c r="K26" s="43"/>
+      <c r="L26" s="43"/>
+      <c r="M26" s="43"/>
+      <c r="N26" s="43"/>
+      <c r="O26" s="43"/>
+      <c r="P26" s="43"/>
+      <c r="Q26" s="44"/>
+      <c r="R26" s="21"/>
+      <c r="S26" s="21"/>
+      <c r="T26" s="21"/>
+      <c r="U26" s="21"/>
+      <c r="V26" s="21"/>
+      <c r="W26" s="21"/>
+      <c r="X26" s="21"/>
+      <c r="Y26" s="21"/>
+      <c r="Z26" s="21"/>
+      <c r="AA26" s="21"/>
+      <c r="AB26" s="21"/>
+      <c r="AC26" s="21"/>
+      <c r="AD26" s="21"/>
+      <c r="AE26" s="21"/>
+      <c r="AF26" s="21"/>
+      <c r="AG26" s="21"/>
+      <c r="AH26" s="21"/>
+      <c r="AI26" s="27"/>
+      <c r="AJ26" s="21"/>
+      <c r="AK26" s="21"/>
+      <c r="AL26" s="21"/>
+      <c r="AM26" s="21"/>
+      <c r="AN26" s="52"/>
+      <c r="AO26" s="52"/>
+      <c r="AP26" s="52"/>
+      <c r="AQ26" s="52"/>
+      <c r="AR26" s="52"/>
+      <c r="AS26" s="52"/>
+      <c r="AT26" s="52"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -3125,7 +3299,8 @@
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="C2:J2"/>
   </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.86614173228346458" right="0.86614173228346458" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
+  <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -3136,8 +3311,8 @@
   </sheetPr>
   <dimension ref="A1:AT26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AR26" sqref="AR26"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="AT26" sqref="R26:AT27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="3.5703125" defaultRowHeight="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3188,92 +3363,92 @@
       <c r="AN1" s="5"/>
     </row>
     <row r="2" spans="1:46" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="8"/>
-      <c r="C2" s="9" t="s">
+      <c r="B2" s="30"/>
+      <c r="C2" s="45" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="10"/>
-      <c r="E2" s="10"/>
-      <c r="F2" s="10"/>
-      <c r="G2" s="10"/>
-      <c r="H2" s="10"/>
-      <c r="I2" s="10"/>
-      <c r="J2" s="11"/>
+      <c r="D2" s="31"/>
+      <c r="E2" s="31"/>
+      <c r="F2" s="31"/>
+      <c r="G2" s="31"/>
+      <c r="H2" s="31"/>
+      <c r="I2" s="31"/>
+      <c r="J2" s="32"/>
       <c r="K2" s="2"/>
       <c r="L2" s="3"/>
-      <c r="M2" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="N2" s="8"/>
-      <c r="O2" s="9" t="s">
+      <c r="M2" s="29" t="s">
         <v>20</v>
       </c>
-      <c r="P2" s="10"/>
-      <c r="Q2" s="10"/>
-      <c r="R2" s="10"/>
-      <c r="S2" s="10"/>
-      <c r="T2" s="10"/>
-      <c r="U2" s="10"/>
-      <c r="V2" s="11"/>
-      <c r="W2" s="12"/>
-      <c r="X2" s="13"/>
-      <c r="Y2" s="13"/>
-      <c r="Z2" s="13"/>
-      <c r="AA2" s="13"/>
-      <c r="AB2" s="13"/>
-      <c r="AC2" s="13"/>
-      <c r="AD2" s="13"/>
-      <c r="AE2" s="13"/>
-      <c r="AF2" s="13"/>
-      <c r="AG2" s="13"/>
-      <c r="AH2" s="13"/>
-      <c r="AI2" s="13"/>
-      <c r="AJ2" s="13"/>
-      <c r="AK2" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="AL2" s="8"/>
-      <c r="AM2" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="AN2" s="10"/>
-      <c r="AO2" s="10"/>
-      <c r="AP2" s="10"/>
-      <c r="AQ2" s="10"/>
-      <c r="AR2" s="10"/>
-      <c r="AS2" s="10"/>
-      <c r="AT2" s="11"/>
+      <c r="N2" s="30"/>
+      <c r="O2" s="45" t="s">
+        <v>17</v>
+      </c>
+      <c r="P2" s="31"/>
+      <c r="Q2" s="31"/>
+      <c r="R2" s="31"/>
+      <c r="S2" s="31"/>
+      <c r="T2" s="31"/>
+      <c r="U2" s="31"/>
+      <c r="V2" s="32"/>
+      <c r="W2" s="7"/>
+      <c r="X2" s="8"/>
+      <c r="Y2" s="8"/>
+      <c r="Z2" s="8"/>
+      <c r="AA2" s="8"/>
+      <c r="AB2" s="8"/>
+      <c r="AC2" s="8"/>
+      <c r="AD2" s="8"/>
+      <c r="AE2" s="8"/>
+      <c r="AF2" s="8"/>
+      <c r="AG2" s="8"/>
+      <c r="AH2" s="8"/>
+      <c r="AI2" s="8"/>
+      <c r="AJ2" s="8"/>
+      <c r="AK2" s="29" t="s">
+        <v>31</v>
+      </c>
+      <c r="AL2" s="30"/>
+      <c r="AM2" s="45" t="s">
+        <v>36</v>
+      </c>
+      <c r="AN2" s="31"/>
+      <c r="AO2" s="31"/>
+      <c r="AP2" s="31"/>
+      <c r="AQ2" s="31"/>
+      <c r="AR2" s="31"/>
+      <c r="AS2" s="31"/>
+      <c r="AT2" s="32"/>
     </row>
     <row r="3" spans="1:46" ht="18.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="14" t="s">
+      <c r="A3" s="33" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="15"/>
-      <c r="C3" s="15"/>
-      <c r="D3" s="15"/>
-      <c r="E3" s="15"/>
-      <c r="F3" s="15"/>
-      <c r="G3" s="15"/>
-      <c r="H3" s="15"/>
-      <c r="I3" s="15"/>
-      <c r="J3" s="16"/>
-      <c r="K3" s="17"/>
-      <c r="L3" s="18"/>
-      <c r="M3" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="N3" s="15"/>
-      <c r="O3" s="15"/>
-      <c r="P3" s="15"/>
-      <c r="Q3" s="15"/>
-      <c r="R3" s="15"/>
-      <c r="S3" s="15"/>
-      <c r="T3" s="15"/>
-      <c r="U3" s="15"/>
-      <c r="V3" s="16"/>
+      <c r="B3" s="34"/>
+      <c r="C3" s="34"/>
+      <c r="D3" s="34"/>
+      <c r="E3" s="34"/>
+      <c r="F3" s="34"/>
+      <c r="G3" s="34"/>
+      <c r="H3" s="34"/>
+      <c r="I3" s="34"/>
+      <c r="J3" s="35"/>
+      <c r="K3" s="9"/>
+      <c r="L3" s="10"/>
+      <c r="M3" s="33" t="s">
+        <v>18</v>
+      </c>
+      <c r="N3" s="34"/>
+      <c r="O3" s="34"/>
+      <c r="P3" s="34"/>
+      <c r="Q3" s="34"/>
+      <c r="R3" s="34"/>
+      <c r="S3" s="34"/>
+      <c r="T3" s="34"/>
+      <c r="U3" s="34"/>
+      <c r="V3" s="35"/>
       <c r="W3" s="3"/>
       <c r="X3" s="2"/>
       <c r="Y3" s="2"/>
@@ -3288,46 +3463,46 @@
       <c r="AH3" s="2"/>
       <c r="AI3" s="2"/>
       <c r="AJ3" s="2"/>
-      <c r="AK3" s="19" t="s">
-        <v>40</v>
-      </c>
-      <c r="AL3" s="20"/>
-      <c r="AM3" s="20"/>
-      <c r="AN3" s="20"/>
-      <c r="AO3" s="20"/>
-      <c r="AP3" s="20"/>
-      <c r="AQ3" s="20"/>
-      <c r="AR3" s="20"/>
-      <c r="AS3" s="20"/>
-      <c r="AT3" s="21"/>
+      <c r="AK3" s="46" t="s">
+        <v>37</v>
+      </c>
+      <c r="AL3" s="47"/>
+      <c r="AM3" s="47"/>
+      <c r="AN3" s="47"/>
+      <c r="AO3" s="47"/>
+      <c r="AP3" s="47"/>
+      <c r="AQ3" s="47"/>
+      <c r="AR3" s="47"/>
+      <c r="AS3" s="47"/>
+      <c r="AT3" s="48"/>
     </row>
     <row r="4" spans="1:46" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="22" t="s">
+      <c r="A4" s="36" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="23"/>
-      <c r="C4" s="23"/>
-      <c r="D4" s="23"/>
-      <c r="E4" s="23"/>
-      <c r="F4" s="23"/>
-      <c r="G4" s="23"/>
-      <c r="H4" s="23"/>
-      <c r="I4" s="23"/>
-      <c r="J4" s="24"/>
-      <c r="K4" s="25"/>
+      <c r="B4" s="37"/>
+      <c r="C4" s="37"/>
+      <c r="D4" s="37"/>
+      <c r="E4" s="37"/>
+      <c r="F4" s="37"/>
+      <c r="G4" s="37"/>
+      <c r="H4" s="37"/>
+      <c r="I4" s="37"/>
+      <c r="J4" s="38"/>
+      <c r="K4" s="11"/>
       <c r="L4" s="3"/>
-      <c r="M4" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="N4" s="23"/>
-      <c r="O4" s="23"/>
-      <c r="P4" s="23"/>
-      <c r="Q4" s="23"/>
-      <c r="R4" s="23"/>
-      <c r="S4" s="23"/>
-      <c r="T4" s="23"/>
-      <c r="U4" s="23"/>
-      <c r="V4" s="24"/>
+      <c r="M4" s="36" t="s">
+        <v>19</v>
+      </c>
+      <c r="N4" s="37"/>
+      <c r="O4" s="37"/>
+      <c r="P4" s="37"/>
+      <c r="Q4" s="37"/>
+      <c r="R4" s="37"/>
+      <c r="S4" s="37"/>
+      <c r="T4" s="37"/>
+      <c r="U4" s="37"/>
+      <c r="V4" s="38"/>
       <c r="W4" s="3"/>
       <c r="X4" s="2"/>
       <c r="Y4" s="2"/>
@@ -3342,29 +3517,29 @@
       <c r="AH4" s="2"/>
       <c r="AI4" s="2"/>
       <c r="AJ4" s="2"/>
-      <c r="AK4" s="26"/>
-      <c r="AL4" s="27"/>
-      <c r="AM4" s="27"/>
-      <c r="AN4" s="27"/>
-      <c r="AO4" s="27"/>
-      <c r="AP4" s="27"/>
-      <c r="AQ4" s="27"/>
-      <c r="AR4" s="27"/>
-      <c r="AS4" s="27"/>
-      <c r="AT4" s="28"/>
+      <c r="AK4" s="49"/>
+      <c r="AL4" s="50"/>
+      <c r="AM4" s="50"/>
+      <c r="AN4" s="50"/>
+      <c r="AO4" s="50"/>
+      <c r="AP4" s="50"/>
+      <c r="AQ4" s="50"/>
+      <c r="AR4" s="50"/>
+      <c r="AS4" s="50"/>
+      <c r="AT4" s="51"/>
     </row>
     <row r="5" spans="1:46" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="29"/>
-      <c r="B5" s="29"/>
-      <c r="C5" s="29"/>
-      <c r="D5" s="29"/>
-      <c r="E5" s="29"/>
-      <c r="F5" s="29"/>
-      <c r="G5" s="29"/>
-      <c r="H5" s="29"/>
-      <c r="I5" s="29"/>
+      <c r="A5" s="12"/>
+      <c r="B5" s="12"/>
+      <c r="C5" s="12"/>
+      <c r="D5" s="12"/>
+      <c r="E5" s="12"/>
+      <c r="F5" s="12"/>
+      <c r="G5" s="12"/>
+      <c r="H5" s="12"/>
+      <c r="I5" s="12"/>
       <c r="J5" s="2"/>
-      <c r="K5" s="25"/>
+      <c r="K5" s="11"/>
       <c r="L5" s="3"/>
       <c r="M5" s="3"/>
       <c r="N5" s="3"/>
@@ -3406,50 +3581,50 @@
       <c r="H6" s="2"/>
       <c r="I6" s="2"/>
       <c r="J6" s="2"/>
-      <c r="K6" s="25"/>
-      <c r="L6" s="30"/>
-      <c r="M6" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="N6" s="8"/>
-      <c r="O6" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="P6" s="10"/>
-      <c r="Q6" s="10"/>
-      <c r="R6" s="10"/>
-      <c r="S6" s="10"/>
-      <c r="T6" s="10"/>
-      <c r="U6" s="10"/>
-      <c r="V6" s="11"/>
-      <c r="W6" s="12"/>
-      <c r="X6" s="13"/>
-      <c r="Y6" s="13"/>
-      <c r="Z6" s="13"/>
-      <c r="AA6" s="13"/>
-      <c r="AB6" s="13"/>
-      <c r="AC6" s="13"/>
-      <c r="AD6" s="13"/>
-      <c r="AE6" s="13"/>
-      <c r="AF6" s="13"/>
-      <c r="AG6" s="13"/>
-      <c r="AH6" s="13"/>
-      <c r="AI6" s="13"/>
-      <c r="AJ6" s="13"/>
-      <c r="AK6" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="AL6" s="8"/>
-      <c r="AM6" s="9" t="s">
-        <v>41</v>
-      </c>
-      <c r="AN6" s="10"/>
-      <c r="AO6" s="10"/>
-      <c r="AP6" s="10"/>
-      <c r="AQ6" s="10"/>
-      <c r="AR6" s="10"/>
-      <c r="AS6" s="10"/>
-      <c r="AT6" s="11"/>
+      <c r="K6" s="11"/>
+      <c r="L6" s="13"/>
+      <c r="M6" s="29" t="s">
+        <v>16</v>
+      </c>
+      <c r="N6" s="30"/>
+      <c r="O6" s="45" t="s">
+        <v>21</v>
+      </c>
+      <c r="P6" s="31"/>
+      <c r="Q6" s="31"/>
+      <c r="R6" s="31"/>
+      <c r="S6" s="31"/>
+      <c r="T6" s="31"/>
+      <c r="U6" s="31"/>
+      <c r="V6" s="32"/>
+      <c r="W6" s="7"/>
+      <c r="X6" s="8"/>
+      <c r="Y6" s="8"/>
+      <c r="Z6" s="8"/>
+      <c r="AA6" s="8"/>
+      <c r="AB6" s="8"/>
+      <c r="AC6" s="8"/>
+      <c r="AD6" s="8"/>
+      <c r="AE6" s="8"/>
+      <c r="AF6" s="8"/>
+      <c r="AG6" s="8"/>
+      <c r="AH6" s="8"/>
+      <c r="AI6" s="8"/>
+      <c r="AJ6" s="8"/>
+      <c r="AK6" s="29" t="s">
+        <v>32</v>
+      </c>
+      <c r="AL6" s="30"/>
+      <c r="AM6" s="45" t="s">
+        <v>38</v>
+      </c>
+      <c r="AN6" s="31"/>
+      <c r="AO6" s="31"/>
+      <c r="AP6" s="31"/>
+      <c r="AQ6" s="31"/>
+      <c r="AR6" s="31"/>
+      <c r="AS6" s="31"/>
+      <c r="AT6" s="32"/>
     </row>
     <row r="7" spans="1:46" ht="18.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
@@ -3462,20 +3637,20 @@
       <c r="H7" s="2"/>
       <c r="I7" s="2"/>
       <c r="J7" s="2"/>
-      <c r="K7" s="25"/>
+      <c r="K7" s="11"/>
       <c r="L7" s="3"/>
-      <c r="M7" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="N7" s="15"/>
-      <c r="O7" s="15"/>
-      <c r="P7" s="15"/>
-      <c r="Q7" s="15"/>
-      <c r="R7" s="15"/>
-      <c r="S7" s="15"/>
-      <c r="T7" s="15"/>
-      <c r="U7" s="15"/>
-      <c r="V7" s="16"/>
+      <c r="M7" s="33" t="s">
+        <v>22</v>
+      </c>
+      <c r="N7" s="34"/>
+      <c r="O7" s="34"/>
+      <c r="P7" s="34"/>
+      <c r="Q7" s="34"/>
+      <c r="R7" s="34"/>
+      <c r="S7" s="34"/>
+      <c r="T7" s="34"/>
+      <c r="U7" s="34"/>
+      <c r="V7" s="35"/>
       <c r="W7" s="3"/>
       <c r="X7" s="2"/>
       <c r="Y7" s="2"/>
@@ -3490,18 +3665,18 @@
       <c r="AH7" s="2"/>
       <c r="AI7" s="2"/>
       <c r="AJ7" s="2"/>
-      <c r="AK7" s="14" t="s">
-        <v>42</v>
-      </c>
-      <c r="AL7" s="15"/>
-      <c r="AM7" s="15"/>
-      <c r="AN7" s="15"/>
-      <c r="AO7" s="15"/>
-      <c r="AP7" s="15"/>
-      <c r="AQ7" s="15"/>
-      <c r="AR7" s="15"/>
-      <c r="AS7" s="15"/>
-      <c r="AT7" s="16"/>
+      <c r="AK7" s="33" t="s">
+        <v>39</v>
+      </c>
+      <c r="AL7" s="34"/>
+      <c r="AM7" s="34"/>
+      <c r="AN7" s="34"/>
+      <c r="AO7" s="34"/>
+      <c r="AP7" s="34"/>
+      <c r="AQ7" s="34"/>
+      <c r="AR7" s="34"/>
+      <c r="AS7" s="34"/>
+      <c r="AT7" s="35"/>
     </row>
     <row r="8" spans="1:46" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1"/>
@@ -3514,18 +3689,18 @@
       <c r="H8" s="2"/>
       <c r="I8" s="2"/>
       <c r="J8" s="2"/>
-      <c r="K8" s="25"/>
+      <c r="K8" s="11"/>
       <c r="L8" s="3"/>
-      <c r="M8" s="22"/>
-      <c r="N8" s="23"/>
-      <c r="O8" s="23"/>
-      <c r="P8" s="23"/>
-      <c r="Q8" s="23"/>
-      <c r="R8" s="23"/>
-      <c r="S8" s="23"/>
-      <c r="T8" s="23"/>
-      <c r="U8" s="23"/>
-      <c r="V8" s="24"/>
+      <c r="M8" s="36"/>
+      <c r="N8" s="37"/>
+      <c r="O8" s="37"/>
+      <c r="P8" s="37"/>
+      <c r="Q8" s="37"/>
+      <c r="R8" s="37"/>
+      <c r="S8" s="37"/>
+      <c r="T8" s="37"/>
+      <c r="U8" s="37"/>
+      <c r="V8" s="38"/>
       <c r="W8" s="3"/>
       <c r="X8" s="2"/>
       <c r="Y8" s="2"/>
@@ -3540,19 +3715,19 @@
       <c r="AH8" s="2"/>
       <c r="AI8" s="2"/>
       <c r="AJ8" s="2"/>
-      <c r="AK8" s="26"/>
-      <c r="AL8" s="27"/>
-      <c r="AM8" s="27"/>
-      <c r="AN8" s="27"/>
-      <c r="AO8" s="27"/>
-      <c r="AP8" s="27"/>
-      <c r="AQ8" s="27"/>
-      <c r="AR8" s="27"/>
-      <c r="AS8" s="27"/>
-      <c r="AT8" s="28"/>
+      <c r="AK8" s="49"/>
+      <c r="AL8" s="50"/>
+      <c r="AM8" s="50"/>
+      <c r="AN8" s="50"/>
+      <c r="AO8" s="50"/>
+      <c r="AP8" s="50"/>
+      <c r="AQ8" s="50"/>
+      <c r="AR8" s="50"/>
+      <c r="AS8" s="50"/>
+      <c r="AT8" s="51"/>
     </row>
     <row r="9" spans="1:46" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="K9" s="31"/>
+      <c r="K9" s="14"/>
       <c r="L9" s="3"/>
       <c r="M9" s="3"/>
       <c r="N9" s="3"/>
@@ -3584,66 +3759,66 @@
       <c r="AN9" s="5"/>
     </row>
     <row r="10" spans="1:46" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="K10" s="31"/>
+      <c r="K10" s="14"/>
       <c r="L10" s="3"/>
-      <c r="M10" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="N10" s="8"/>
-      <c r="O10" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="P10" s="10"/>
-      <c r="Q10" s="10"/>
-      <c r="R10" s="10"/>
-      <c r="S10" s="10"/>
-      <c r="T10" s="10"/>
-      <c r="U10" s="10"/>
-      <c r="V10" s="11"/>
-      <c r="W10" s="12"/>
-      <c r="X10" s="13"/>
-      <c r="Y10" s="13"/>
-      <c r="Z10" s="13"/>
-      <c r="AA10" s="13"/>
-      <c r="AB10" s="13"/>
-      <c r="AC10" s="13"/>
-      <c r="AD10" s="13"/>
-      <c r="AE10" s="13"/>
-      <c r="AF10" s="13"/>
-      <c r="AG10" s="13"/>
-      <c r="AH10" s="13"/>
-      <c r="AI10" s="13"/>
-      <c r="AJ10" s="13"/>
-      <c r="AK10" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="AL10" s="8"/>
-      <c r="AM10" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="AN10" s="10"/>
-      <c r="AO10" s="10"/>
-      <c r="AP10" s="10"/>
-      <c r="AQ10" s="10"/>
-      <c r="AR10" s="10"/>
-      <c r="AS10" s="10"/>
-      <c r="AT10" s="11"/>
+      <c r="M10" s="29" t="s">
+        <v>23</v>
+      </c>
+      <c r="N10" s="30"/>
+      <c r="O10" s="45" t="s">
+        <v>24</v>
+      </c>
+      <c r="P10" s="31"/>
+      <c r="Q10" s="31"/>
+      <c r="R10" s="31"/>
+      <c r="S10" s="31"/>
+      <c r="T10" s="31"/>
+      <c r="U10" s="31"/>
+      <c r="V10" s="32"/>
+      <c r="W10" s="7"/>
+      <c r="X10" s="8"/>
+      <c r="Y10" s="8"/>
+      <c r="Z10" s="8"/>
+      <c r="AA10" s="8"/>
+      <c r="AB10" s="8"/>
+      <c r="AC10" s="8"/>
+      <c r="AD10" s="8"/>
+      <c r="AE10" s="8"/>
+      <c r="AF10" s="8"/>
+      <c r="AG10" s="8"/>
+      <c r="AH10" s="8"/>
+      <c r="AI10" s="8"/>
+      <c r="AJ10" s="8"/>
+      <c r="AK10" s="29" t="s">
+        <v>33</v>
+      </c>
+      <c r="AL10" s="30"/>
+      <c r="AM10" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="AN10" s="31"/>
+      <c r="AO10" s="31"/>
+      <c r="AP10" s="31"/>
+      <c r="AQ10" s="31"/>
+      <c r="AR10" s="31"/>
+      <c r="AS10" s="31"/>
+      <c r="AT10" s="32"/>
     </row>
     <row r="11" spans="1:46" ht="18.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="K11" s="31"/>
-      <c r="L11" s="32"/>
-      <c r="M11" s="14" t="s">
-        <v>28</v>
-      </c>
-      <c r="N11" s="15"/>
-      <c r="O11" s="15"/>
-      <c r="P11" s="15"/>
-      <c r="Q11" s="15"/>
-      <c r="R11" s="15"/>
-      <c r="S11" s="15"/>
-      <c r="T11" s="15"/>
-      <c r="U11" s="15"/>
-      <c r="V11" s="16"/>
+      <c r="K11" s="14"/>
+      <c r="L11" s="15"/>
+      <c r="M11" s="33" t="s">
+        <v>25</v>
+      </c>
+      <c r="N11" s="34"/>
+      <c r="O11" s="34"/>
+      <c r="P11" s="34"/>
+      <c r="Q11" s="34"/>
+      <c r="R11" s="34"/>
+      <c r="S11" s="34"/>
+      <c r="T11" s="34"/>
+      <c r="U11" s="34"/>
+      <c r="V11" s="35"/>
       <c r="W11" s="3"/>
       <c r="X11" s="2"/>
       <c r="Y11" s="2"/>
@@ -3658,30 +3833,30 @@
       <c r="AH11" s="2"/>
       <c r="AI11" s="2"/>
       <c r="AJ11" s="2"/>
-      <c r="AK11" s="14"/>
-      <c r="AL11" s="15"/>
-      <c r="AM11" s="15"/>
-      <c r="AN11" s="15"/>
-      <c r="AO11" s="15"/>
-      <c r="AP11" s="15"/>
-      <c r="AQ11" s="15"/>
-      <c r="AR11" s="15"/>
-      <c r="AS11" s="15"/>
-      <c r="AT11" s="16"/>
+      <c r="AK11" s="33"/>
+      <c r="AL11" s="34"/>
+      <c r="AM11" s="34"/>
+      <c r="AN11" s="34"/>
+      <c r="AO11" s="34"/>
+      <c r="AP11" s="34"/>
+      <c r="AQ11" s="34"/>
+      <c r="AR11" s="34"/>
+      <c r="AS11" s="34"/>
+      <c r="AT11" s="35"/>
     </row>
     <row r="12" spans="1:46" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="K12" s="31"/>
+      <c r="K12" s="14"/>
       <c r="L12" s="3"/>
-      <c r="M12" s="22"/>
-      <c r="N12" s="23"/>
-      <c r="O12" s="23"/>
-      <c r="P12" s="23"/>
-      <c r="Q12" s="23"/>
-      <c r="R12" s="23"/>
-      <c r="S12" s="23"/>
-      <c r="T12" s="23"/>
-      <c r="U12" s="23"/>
-      <c r="V12" s="24"/>
+      <c r="M12" s="36"/>
+      <c r="N12" s="37"/>
+      <c r="O12" s="37"/>
+      <c r="P12" s="37"/>
+      <c r="Q12" s="37"/>
+      <c r="R12" s="37"/>
+      <c r="S12" s="37"/>
+      <c r="T12" s="37"/>
+      <c r="U12" s="37"/>
+      <c r="V12" s="38"/>
       <c r="W12" s="3"/>
       <c r="X12" s="2"/>
       <c r="Y12" s="2"/>
@@ -3696,19 +3871,19 @@
       <c r="AH12" s="2"/>
       <c r="AI12" s="2"/>
       <c r="AJ12" s="2"/>
-      <c r="AK12" s="22"/>
-      <c r="AL12" s="23"/>
-      <c r="AM12" s="23"/>
-      <c r="AN12" s="23"/>
-      <c r="AO12" s="23"/>
-      <c r="AP12" s="23"/>
-      <c r="AQ12" s="23"/>
-      <c r="AR12" s="23"/>
-      <c r="AS12" s="23"/>
-      <c r="AT12" s="24"/>
+      <c r="AK12" s="36"/>
+      <c r="AL12" s="37"/>
+      <c r="AM12" s="37"/>
+      <c r="AN12" s="37"/>
+      <c r="AO12" s="37"/>
+      <c r="AP12" s="37"/>
+      <c r="AQ12" s="37"/>
+      <c r="AR12" s="37"/>
+      <c r="AS12" s="37"/>
+      <c r="AT12" s="38"/>
     </row>
     <row r="13" spans="1:46" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="K13" s="31"/>
+      <c r="K13" s="14"/>
       <c r="L13" s="3"/>
       <c r="M13" s="3"/>
       <c r="N13" s="3"/>
@@ -3740,118 +3915,118 @@
       <c r="AN13" s="5"/>
     </row>
     <row r="14" spans="1:46" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="29"/>
-      <c r="B14" s="29"/>
-      <c r="C14" s="29"/>
-      <c r="D14" s="29"/>
-      <c r="E14" s="29"/>
-      <c r="F14" s="29"/>
-      <c r="G14" s="29"/>
-      <c r="H14" s="29"/>
-      <c r="I14" s="29"/>
+      <c r="A14" s="12"/>
+      <c r="B14" s="12"/>
+      <c r="C14" s="12"/>
+      <c r="D14" s="12"/>
+      <c r="E14" s="12"/>
+      <c r="F14" s="12"/>
+      <c r="G14" s="12"/>
+      <c r="H14" s="12"/>
+      <c r="I14" s="12"/>
       <c r="J14" s="2"/>
-      <c r="K14" s="25"/>
+      <c r="K14" s="11"/>
       <c r="L14" s="3"/>
-      <c r="M14" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="N14" s="8"/>
-      <c r="O14" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="P14" s="10"/>
-      <c r="Q14" s="10"/>
-      <c r="R14" s="10"/>
-      <c r="S14" s="10"/>
-      <c r="T14" s="10"/>
-      <c r="U14" s="10"/>
-      <c r="V14" s="11"/>
-      <c r="W14" s="12"/>
-      <c r="X14" s="13"/>
-      <c r="Y14" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="Z14" s="8"/>
-      <c r="AA14" s="9" t="s">
+      <c r="M14" s="29" t="s">
+        <v>26</v>
+      </c>
+      <c r="N14" s="30"/>
+      <c r="O14" s="45" t="s">
+        <v>41</v>
+      </c>
+      <c r="P14" s="31"/>
+      <c r="Q14" s="31"/>
+      <c r="R14" s="31"/>
+      <c r="S14" s="31"/>
+      <c r="T14" s="31"/>
+      <c r="U14" s="31"/>
+      <c r="V14" s="32"/>
+      <c r="W14" s="7"/>
+      <c r="X14" s="8"/>
+      <c r="Y14" s="29" t="s">
+        <v>46</v>
+      </c>
+      <c r="Z14" s="30"/>
+      <c r="AA14" s="45" t="s">
+        <v>42</v>
+      </c>
+      <c r="AB14" s="31"/>
+      <c r="AC14" s="31"/>
+      <c r="AD14" s="31"/>
+      <c r="AE14" s="31"/>
+      <c r="AF14" s="31"/>
+      <c r="AG14" s="31"/>
+      <c r="AH14" s="32"/>
+      <c r="AI14" s="16"/>
+      <c r="AJ14" s="8"/>
+      <c r="AK14" s="29" t="s">
         <v>45</v>
       </c>
-      <c r="AB14" s="10"/>
-      <c r="AC14" s="10"/>
-      <c r="AD14" s="10"/>
-      <c r="AE14" s="10"/>
-      <c r="AF14" s="10"/>
-      <c r="AG14" s="10"/>
-      <c r="AH14" s="11"/>
-      <c r="AI14" s="33"/>
-      <c r="AJ14" s="13"/>
-      <c r="AK14" s="7" t="s">
+      <c r="AL14" s="30"/>
+      <c r="AM14" s="45" t="s">
         <v>48</v>
       </c>
-      <c r="AL14" s="8"/>
-      <c r="AM14" s="9" t="s">
-        <v>51</v>
-      </c>
-      <c r="AN14" s="10"/>
-      <c r="AO14" s="10"/>
-      <c r="AP14" s="10"/>
-      <c r="AQ14" s="10"/>
-      <c r="AR14" s="10"/>
-      <c r="AS14" s="10"/>
-      <c r="AT14" s="11"/>
+      <c r="AN14" s="31"/>
+      <c r="AO14" s="31"/>
+      <c r="AP14" s="31"/>
+      <c r="AQ14" s="31"/>
+      <c r="AR14" s="31"/>
+      <c r="AS14" s="31"/>
+      <c r="AT14" s="32"/>
     </row>
     <row r="15" spans="1:46" ht="18.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="29"/>
-      <c r="B15" s="29"/>
-      <c r="C15" s="29"/>
-      <c r="D15" s="29"/>
-      <c r="E15" s="29"/>
-      <c r="F15" s="29"/>
+      <c r="A15" s="12"/>
+      <c r="B15" s="12"/>
+      <c r="C15" s="12"/>
+      <c r="D15" s="12"/>
+      <c r="E15" s="12"/>
+      <c r="F15" s="12"/>
       <c r="G15" s="3"/>
       <c r="H15" s="3"/>
       <c r="I15" s="2"/>
       <c r="J15" s="2"/>
-      <c r="K15" s="25"/>
-      <c r="L15" s="34"/>
-      <c r="M15" s="14" t="s">
-        <v>47</v>
-      </c>
-      <c r="N15" s="15"/>
-      <c r="O15" s="15"/>
-      <c r="P15" s="15"/>
-      <c r="Q15" s="15"/>
-      <c r="R15" s="15"/>
-      <c r="S15" s="15"/>
-      <c r="T15" s="15"/>
-      <c r="U15" s="15"/>
-      <c r="V15" s="16"/>
-      <c r="W15" s="35"/>
+      <c r="K15" s="11"/>
+      <c r="L15" s="17"/>
+      <c r="M15" s="33" t="s">
+        <v>44</v>
+      </c>
+      <c r="N15" s="34"/>
+      <c r="O15" s="34"/>
+      <c r="P15" s="34"/>
+      <c r="Q15" s="34"/>
+      <c r="R15" s="34"/>
+      <c r="S15" s="34"/>
+      <c r="T15" s="34"/>
+      <c r="U15" s="34"/>
+      <c r="V15" s="35"/>
+      <c r="W15" s="18"/>
       <c r="X15" s="2"/>
-      <c r="Y15" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="Z15" s="15"/>
-      <c r="AA15" s="15"/>
-      <c r="AB15" s="15"/>
-      <c r="AC15" s="15"/>
-      <c r="AD15" s="15"/>
-      <c r="AE15" s="15"/>
-      <c r="AF15" s="15"/>
-      <c r="AG15" s="15"/>
-      <c r="AH15" s="16"/>
+      <c r="Y15" s="33" t="s">
+        <v>43</v>
+      </c>
+      <c r="Z15" s="34"/>
+      <c r="AA15" s="34"/>
+      <c r="AB15" s="34"/>
+      <c r="AC15" s="34"/>
+      <c r="AD15" s="34"/>
+      <c r="AE15" s="34"/>
+      <c r="AF15" s="34"/>
+      <c r="AG15" s="34"/>
+      <c r="AH15" s="35"/>
       <c r="AI15" s="2"/>
       <c r="AJ15" s="2"/>
-      <c r="AK15" s="14" t="s">
-        <v>52</v>
-      </c>
-      <c r="AL15" s="15"/>
-      <c r="AM15" s="15"/>
-      <c r="AN15" s="15"/>
-      <c r="AO15" s="15"/>
-      <c r="AP15" s="15"/>
-      <c r="AQ15" s="15"/>
-      <c r="AR15" s="15"/>
-      <c r="AS15" s="15"/>
-      <c r="AT15" s="16"/>
+      <c r="AK15" s="33" t="s">
+        <v>49</v>
+      </c>
+      <c r="AL15" s="34"/>
+      <c r="AM15" s="34"/>
+      <c r="AN15" s="34"/>
+      <c r="AO15" s="34"/>
+      <c r="AP15" s="34"/>
+      <c r="AQ15" s="34"/>
+      <c r="AR15" s="34"/>
+      <c r="AS15" s="34"/>
+      <c r="AT15" s="35"/>
     </row>
     <row r="16" spans="1:46" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="1"/>
@@ -3864,44 +4039,44 @@
       <c r="H16" s="2"/>
       <c r="I16" s="2"/>
       <c r="J16" s="2"/>
-      <c r="K16" s="25"/>
+      <c r="K16" s="11"/>
       <c r="L16" s="3"/>
-      <c r="M16" s="22"/>
-      <c r="N16" s="23"/>
-      <c r="O16" s="23"/>
-      <c r="P16" s="23"/>
-      <c r="Q16" s="23"/>
-      <c r="R16" s="23"/>
-      <c r="S16" s="23"/>
-      <c r="T16" s="23"/>
-      <c r="U16" s="23"/>
-      <c r="V16" s="24"/>
-      <c r="W16" s="36"/>
+      <c r="M16" s="36"/>
+      <c r="N16" s="37"/>
+      <c r="O16" s="37"/>
+      <c r="P16" s="37"/>
+      <c r="Q16" s="37"/>
+      <c r="R16" s="37"/>
+      <c r="S16" s="37"/>
+      <c r="T16" s="37"/>
+      <c r="U16" s="37"/>
+      <c r="V16" s="38"/>
+      <c r="W16" s="19"/>
       <c r="X16" s="2"/>
-      <c r="Y16" s="22"/>
-      <c r="Z16" s="23"/>
-      <c r="AA16" s="23"/>
-      <c r="AB16" s="23"/>
-      <c r="AC16" s="23"/>
-      <c r="AD16" s="23"/>
-      <c r="AE16" s="23"/>
-      <c r="AF16" s="23"/>
-      <c r="AG16" s="23"/>
-      <c r="AH16" s="24"/>
+      <c r="Y16" s="36"/>
+      <c r="Z16" s="37"/>
+      <c r="AA16" s="37"/>
+      <c r="AB16" s="37"/>
+      <c r="AC16" s="37"/>
+      <c r="AD16" s="37"/>
+      <c r="AE16" s="37"/>
+      <c r="AF16" s="37"/>
+      <c r="AG16" s="37"/>
+      <c r="AH16" s="38"/>
       <c r="AI16" s="2"/>
       <c r="AJ16" s="2"/>
-      <c r="AK16" s="22" t="s">
-        <v>53</v>
-      </c>
-      <c r="AL16" s="23"/>
-      <c r="AM16" s="23"/>
-      <c r="AN16" s="23"/>
-      <c r="AO16" s="23"/>
-      <c r="AP16" s="23"/>
-      <c r="AQ16" s="23"/>
-      <c r="AR16" s="23"/>
-      <c r="AS16" s="23"/>
-      <c r="AT16" s="24"/>
+      <c r="AK16" s="36" t="s">
+        <v>50</v>
+      </c>
+      <c r="AL16" s="37"/>
+      <c r="AM16" s="37"/>
+      <c r="AN16" s="37"/>
+      <c r="AO16" s="37"/>
+      <c r="AP16" s="37"/>
+      <c r="AQ16" s="37"/>
+      <c r="AR16" s="37"/>
+      <c r="AS16" s="37"/>
+      <c r="AT16" s="38"/>
     </row>
     <row r="17" spans="1:46" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="1"/>
@@ -3914,7 +4089,7 @@
       <c r="H17" s="2"/>
       <c r="I17" s="2"/>
       <c r="J17" s="2"/>
-      <c r="K17" s="25"/>
+      <c r="K17" s="11"/>
       <c r="L17" s="3"/>
       <c r="M17" s="3"/>
       <c r="N17" s="3"/>
@@ -3926,7 +4101,7 @@
       <c r="T17" s="3"/>
       <c r="U17" s="3"/>
       <c r="V17" s="3"/>
-      <c r="W17" s="36"/>
+      <c r="W17" s="19"/>
       <c r="X17" s="2"/>
       <c r="Y17" s="2"/>
       <c r="Z17" s="2"/>
@@ -3956,39 +4131,39 @@
       <c r="H18" s="2"/>
       <c r="I18" s="2"/>
       <c r="J18" s="2"/>
-      <c r="K18" s="25"/>
-      <c r="W18" s="36"/>
-      <c r="X18" s="37"/>
-      <c r="Y18" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="Z18" s="8"/>
-      <c r="AA18" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="AB18" s="10"/>
-      <c r="AC18" s="10"/>
-      <c r="AD18" s="10"/>
-      <c r="AE18" s="10"/>
-      <c r="AF18" s="10"/>
-      <c r="AG18" s="10"/>
-      <c r="AH18" s="11"/>
-      <c r="AI18" s="33"/>
-      <c r="AJ18" s="13"/>
-      <c r="AK18" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="AL18" s="8"/>
-      <c r="AM18" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="AN18" s="10"/>
-      <c r="AO18" s="10"/>
-      <c r="AP18" s="10"/>
-      <c r="AQ18" s="10"/>
-      <c r="AR18" s="10"/>
-      <c r="AS18" s="10"/>
-      <c r="AT18" s="11"/>
+      <c r="K18" s="11"/>
+      <c r="W18" s="19"/>
+      <c r="X18" s="20"/>
+      <c r="Y18" s="29" t="s">
+        <v>47</v>
+      </c>
+      <c r="Z18" s="30"/>
+      <c r="AA18" s="45" t="s">
+        <v>51</v>
+      </c>
+      <c r="AB18" s="31"/>
+      <c r="AC18" s="31"/>
+      <c r="AD18" s="31"/>
+      <c r="AE18" s="31"/>
+      <c r="AF18" s="31"/>
+      <c r="AG18" s="31"/>
+      <c r="AH18" s="32"/>
+      <c r="AI18" s="16"/>
+      <c r="AJ18" s="8"/>
+      <c r="AK18" s="29" t="s">
+        <v>35</v>
+      </c>
+      <c r="AL18" s="30"/>
+      <c r="AM18" s="45" t="s">
+        <v>53</v>
+      </c>
+      <c r="AN18" s="31"/>
+      <c r="AO18" s="31"/>
+      <c r="AP18" s="31"/>
+      <c r="AQ18" s="31"/>
+      <c r="AR18" s="31"/>
+      <c r="AS18" s="31"/>
+      <c r="AT18" s="32"/>
     </row>
     <row r="19" spans="1:46" ht="18.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
@@ -4001,35 +4176,35 @@
       <c r="H19" s="2"/>
       <c r="I19" s="2"/>
       <c r="J19" s="2"/>
-      <c r="K19" s="25"/>
+      <c r="K19" s="11"/>
       <c r="W19" s="3"/>
       <c r="X19" s="2"/>
-      <c r="Y19" s="14" t="s">
-        <v>55</v>
-      </c>
-      <c r="Z19" s="15"/>
-      <c r="AA19" s="15"/>
-      <c r="AB19" s="15"/>
-      <c r="AC19" s="15"/>
-      <c r="AD19" s="15"/>
-      <c r="AE19" s="15"/>
-      <c r="AF19" s="15"/>
-      <c r="AG19" s="15"/>
-      <c r="AH19" s="16"/>
+      <c r="Y19" s="33" t="s">
+        <v>52</v>
+      </c>
+      <c r="Z19" s="34"/>
+      <c r="AA19" s="34"/>
+      <c r="AB19" s="34"/>
+      <c r="AC19" s="34"/>
+      <c r="AD19" s="34"/>
+      <c r="AE19" s="34"/>
+      <c r="AF19" s="34"/>
+      <c r="AG19" s="34"/>
+      <c r="AH19" s="35"/>
       <c r="AI19" s="2"/>
       <c r="AJ19" s="2"/>
-      <c r="AK19" s="14" t="s">
-        <v>57</v>
-      </c>
-      <c r="AL19" s="15"/>
-      <c r="AM19" s="15"/>
-      <c r="AN19" s="15"/>
-      <c r="AO19" s="15"/>
-      <c r="AP19" s="15"/>
-      <c r="AQ19" s="15"/>
-      <c r="AR19" s="15"/>
-      <c r="AS19" s="15"/>
-      <c r="AT19" s="16"/>
+      <c r="AK19" s="33" t="s">
+        <v>54</v>
+      </c>
+      <c r="AL19" s="34"/>
+      <c r="AM19" s="34"/>
+      <c r="AN19" s="34"/>
+      <c r="AO19" s="34"/>
+      <c r="AP19" s="34"/>
+      <c r="AQ19" s="34"/>
+      <c r="AR19" s="34"/>
+      <c r="AS19" s="34"/>
+      <c r="AT19" s="35"/>
     </row>
     <row r="20" spans="1:46" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="1"/>
@@ -4042,33 +4217,33 @@
       <c r="H20" s="2"/>
       <c r="I20" s="2"/>
       <c r="J20" s="2"/>
-      <c r="K20" s="25"/>
+      <c r="K20" s="11"/>
       <c r="W20" s="3"/>
       <c r="X20" s="2"/>
-      <c r="Y20" s="22"/>
-      <c r="Z20" s="23"/>
-      <c r="AA20" s="23"/>
-      <c r="AB20" s="23"/>
-      <c r="AC20" s="23"/>
-      <c r="AD20" s="23"/>
-      <c r="AE20" s="23"/>
-      <c r="AF20" s="23"/>
-      <c r="AG20" s="23"/>
-      <c r="AH20" s="24"/>
+      <c r="Y20" s="36"/>
+      <c r="Z20" s="37"/>
+      <c r="AA20" s="37"/>
+      <c r="AB20" s="37"/>
+      <c r="AC20" s="37"/>
+      <c r="AD20" s="37"/>
+      <c r="AE20" s="37"/>
+      <c r="AF20" s="37"/>
+      <c r="AG20" s="37"/>
+      <c r="AH20" s="38"/>
       <c r="AI20" s="2"/>
       <c r="AJ20" s="2"/>
-      <c r="AK20" s="22" t="s">
-        <v>58</v>
-      </c>
-      <c r="AL20" s="23"/>
-      <c r="AM20" s="23"/>
-      <c r="AN20" s="23"/>
-      <c r="AO20" s="23"/>
-      <c r="AP20" s="23"/>
-      <c r="AQ20" s="23"/>
-      <c r="AR20" s="23"/>
-      <c r="AS20" s="23"/>
-      <c r="AT20" s="24"/>
+      <c r="AK20" s="36" t="s">
+        <v>55</v>
+      </c>
+      <c r="AL20" s="37"/>
+      <c r="AM20" s="37"/>
+      <c r="AN20" s="37"/>
+      <c r="AO20" s="37"/>
+      <c r="AP20" s="37"/>
+      <c r="AQ20" s="37"/>
+      <c r="AR20" s="37"/>
+      <c r="AS20" s="37"/>
+      <c r="AT20" s="38"/>
     </row>
     <row r="21" spans="1:46" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="1"/>
@@ -4081,7 +4256,7 @@
       <c r="H21" s="2"/>
       <c r="I21" s="2"/>
       <c r="J21" s="2"/>
-      <c r="K21" s="25"/>
+      <c r="K21" s="11"/>
       <c r="L21" s="3"/>
       <c r="M21" s="3"/>
       <c r="N21" s="3"/>
@@ -4124,49 +4299,49 @@
       <c r="I22" s="2"/>
       <c r="J22" s="2"/>
       <c r="K22" s="2"/>
-      <c r="L22" s="30"/>
-      <c r="M22" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="N22" s="8"/>
-      <c r="O22" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="P22" s="10"/>
-      <c r="Q22" s="10"/>
-      <c r="R22" s="10"/>
-      <c r="S22" s="10"/>
-      <c r="T22" s="10"/>
-      <c r="U22" s="10"/>
-      <c r="V22" s="11"/>
-      <c r="W22" s="12"/>
-      <c r="X22" s="13"/>
-      <c r="Y22" s="13"/>
-      <c r="Z22" s="13"/>
-      <c r="AA22" s="13"/>
-      <c r="AB22" s="13"/>
-      <c r="AC22" s="13"/>
-      <c r="AD22" s="13"/>
-      <c r="AE22" s="13"/>
-      <c r="AF22" s="13"/>
-      <c r="AG22" s="13"/>
-      <c r="AH22" s="13"/>
-      <c r="AI22" s="13"/>
-      <c r="AJ22" s="13"/>
-      <c r="AK22" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="AL22" s="8"/>
-      <c r="AM22" s="9" t="s">
-        <v>59</v>
-      </c>
-      <c r="AN22" s="10"/>
-      <c r="AO22" s="10"/>
-      <c r="AP22" s="10"/>
-      <c r="AQ22" s="10"/>
-      <c r="AR22" s="10"/>
-      <c r="AS22" s="10"/>
-      <c r="AT22" s="11"/>
+      <c r="L22" s="13"/>
+      <c r="M22" s="29" t="s">
+        <v>27</v>
+      </c>
+      <c r="N22" s="30"/>
+      <c r="O22" s="45" t="s">
+        <v>28</v>
+      </c>
+      <c r="P22" s="31"/>
+      <c r="Q22" s="31"/>
+      <c r="R22" s="31"/>
+      <c r="S22" s="31"/>
+      <c r="T22" s="31"/>
+      <c r="U22" s="31"/>
+      <c r="V22" s="32"/>
+      <c r="W22" s="7"/>
+      <c r="X22" s="8"/>
+      <c r="Y22" s="8"/>
+      <c r="Z22" s="8"/>
+      <c r="AA22" s="8"/>
+      <c r="AB22" s="8"/>
+      <c r="AC22" s="8"/>
+      <c r="AD22" s="8"/>
+      <c r="AE22" s="8"/>
+      <c r="AF22" s="8"/>
+      <c r="AG22" s="8"/>
+      <c r="AH22" s="8"/>
+      <c r="AI22" s="8"/>
+      <c r="AJ22" s="8"/>
+      <c r="AK22" s="29" t="s">
+        <v>34</v>
+      </c>
+      <c r="AL22" s="30"/>
+      <c r="AM22" s="45" t="s">
+        <v>56</v>
+      </c>
+      <c r="AN22" s="31"/>
+      <c r="AO22" s="31"/>
+      <c r="AP22" s="31"/>
+      <c r="AQ22" s="31"/>
+      <c r="AR22" s="31"/>
+      <c r="AS22" s="31"/>
+      <c r="AT22" s="32"/>
     </row>
     <row r="23" spans="1:46" ht="18.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
@@ -4181,18 +4356,18 @@
       <c r="J23" s="2"/>
       <c r="K23" s="2"/>
       <c r="L23" s="3"/>
-      <c r="M23" s="14" t="s">
-        <v>32</v>
-      </c>
-      <c r="N23" s="15"/>
-      <c r="O23" s="15"/>
-      <c r="P23" s="15"/>
-      <c r="Q23" s="15"/>
-      <c r="R23" s="15"/>
-      <c r="S23" s="15"/>
-      <c r="T23" s="15"/>
-      <c r="U23" s="15"/>
-      <c r="V23" s="16"/>
+      <c r="M23" s="33" t="s">
+        <v>29</v>
+      </c>
+      <c r="N23" s="34"/>
+      <c r="O23" s="34"/>
+      <c r="P23" s="34"/>
+      <c r="Q23" s="34"/>
+      <c r="R23" s="34"/>
+      <c r="S23" s="34"/>
+      <c r="T23" s="34"/>
+      <c r="U23" s="34"/>
+      <c r="V23" s="35"/>
       <c r="W23" s="2"/>
       <c r="X23" s="2"/>
       <c r="Y23" s="2"/>
@@ -4207,18 +4382,18 @@
       <c r="AH23" s="2"/>
       <c r="AI23" s="2"/>
       <c r="AJ23" s="2"/>
-      <c r="AK23" s="14" t="s">
-        <v>60</v>
-      </c>
-      <c r="AL23" s="15"/>
-      <c r="AM23" s="15"/>
-      <c r="AN23" s="15"/>
-      <c r="AO23" s="15"/>
-      <c r="AP23" s="15"/>
-      <c r="AQ23" s="15"/>
-      <c r="AR23" s="15"/>
-      <c r="AS23" s="15"/>
-      <c r="AT23" s="16"/>
+      <c r="AK23" s="33" t="s">
+        <v>57</v>
+      </c>
+      <c r="AL23" s="34"/>
+      <c r="AM23" s="34"/>
+      <c r="AN23" s="34"/>
+      <c r="AO23" s="34"/>
+      <c r="AP23" s="34"/>
+      <c r="AQ23" s="34"/>
+      <c r="AR23" s="34"/>
+      <c r="AS23" s="34"/>
+      <c r="AT23" s="35"/>
     </row>
     <row r="24" spans="1:46" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="1"/>
@@ -4233,18 +4408,18 @@
       <c r="J24" s="2"/>
       <c r="K24" s="2"/>
       <c r="L24" s="3"/>
-      <c r="M24" s="22" t="s">
-        <v>33</v>
-      </c>
-      <c r="N24" s="23"/>
-      <c r="O24" s="23"/>
-      <c r="P24" s="23"/>
-      <c r="Q24" s="23"/>
-      <c r="R24" s="23"/>
-      <c r="S24" s="23"/>
-      <c r="T24" s="23"/>
-      <c r="U24" s="23"/>
-      <c r="V24" s="24"/>
+      <c r="M24" s="36" t="s">
+        <v>30</v>
+      </c>
+      <c r="N24" s="37"/>
+      <c r="O24" s="37"/>
+      <c r="P24" s="37"/>
+      <c r="Q24" s="37"/>
+      <c r="R24" s="37"/>
+      <c r="S24" s="37"/>
+      <c r="T24" s="37"/>
+      <c r="U24" s="37"/>
+      <c r="V24" s="38"/>
       <c r="W24" s="2"/>
       <c r="X24" s="2"/>
       <c r="Y24" s="2"/>
@@ -4259,37 +4434,37 @@
       <c r="AH24" s="2"/>
       <c r="AI24" s="2"/>
       <c r="AJ24" s="2"/>
-      <c r="AK24" s="22"/>
-      <c r="AL24" s="23"/>
-      <c r="AM24" s="23"/>
-      <c r="AN24" s="23"/>
-      <c r="AO24" s="23"/>
-      <c r="AP24" s="23"/>
-      <c r="AQ24" s="23"/>
-      <c r="AR24" s="23"/>
-      <c r="AS24" s="23"/>
-      <c r="AT24" s="24"/>
+      <c r="AK24" s="36"/>
+      <c r="AL24" s="37"/>
+      <c r="AM24" s="37"/>
+      <c r="AN24" s="37"/>
+      <c r="AO24" s="37"/>
+      <c r="AP24" s="37"/>
+      <c r="AQ24" s="37"/>
+      <c r="AR24" s="37"/>
+      <c r="AS24" s="37"/>
+      <c r="AT24" s="38"/>
     </row>
     <row r="25" spans="1:46" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="38" t="s">
-        <v>17</v>
-      </c>
-      <c r="B25" s="39"/>
-      <c r="C25" s="39"/>
-      <c r="D25" s="39"/>
-      <c r="E25" s="39"/>
-      <c r="F25" s="39"/>
-      <c r="G25" s="39"/>
-      <c r="H25" s="39"/>
-      <c r="I25" s="39"/>
-      <c r="J25" s="39"/>
-      <c r="K25" s="39"/>
-      <c r="L25" s="39"/>
-      <c r="M25" s="39"/>
-      <c r="N25" s="39"/>
-      <c r="O25" s="39"/>
-      <c r="P25" s="39"/>
-      <c r="Q25" s="40"/>
+      <c r="A25" s="39" t="s">
+        <v>14</v>
+      </c>
+      <c r="B25" s="40"/>
+      <c r="C25" s="40"/>
+      <c r="D25" s="40"/>
+      <c r="E25" s="40"/>
+      <c r="F25" s="40"/>
+      <c r="G25" s="40"/>
+      <c r="H25" s="40"/>
+      <c r="I25" s="40"/>
+      <c r="J25" s="40"/>
+      <c r="K25" s="40"/>
+      <c r="L25" s="40"/>
+      <c r="M25" s="40"/>
+      <c r="N25" s="40"/>
+      <c r="O25" s="40"/>
+      <c r="P25" s="40"/>
+      <c r="Q25" s="41"/>
       <c r="R25" s="2"/>
       <c r="S25" s="2"/>
       <c r="T25" s="2"/>
@@ -4315,54 +4490,55 @@
       <c r="AN25" s="5"/>
     </row>
     <row r="26" spans="1:46" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="41"/>
-      <c r="B26" s="42"/>
-      <c r="C26" s="42"/>
-      <c r="D26" s="42"/>
-      <c r="E26" s="42"/>
-      <c r="F26" s="42"/>
-      <c r="G26" s="42"/>
-      <c r="H26" s="42"/>
-      <c r="I26" s="42"/>
-      <c r="J26" s="42"/>
-      <c r="K26" s="42"/>
-      <c r="L26" s="42"/>
-      <c r="M26" s="42"/>
-      <c r="N26" s="42"/>
-      <c r="O26" s="42"/>
-      <c r="P26" s="42"/>
-      <c r="Q26" s="43"/>
-      <c r="R26" s="44"/>
-      <c r="S26" s="44"/>
-      <c r="T26" s="44"/>
-      <c r="U26" s="44"/>
-      <c r="V26" s="44"/>
-      <c r="W26" s="44"/>
-      <c r="X26" s="44"/>
-      <c r="Y26" s="44"/>
-      <c r="Z26" s="44"/>
-      <c r="AA26" s="44"/>
-      <c r="AB26" s="44"/>
-      <c r="AC26" s="44"/>
-      <c r="AD26" s="44"/>
-      <c r="AE26" s="44"/>
-      <c r="AF26" s="44"/>
-      <c r="AG26" s="44"/>
-      <c r="AH26" s="44"/>
-      <c r="AI26" s="44"/>
-      <c r="AJ26" s="44"/>
-      <c r="AK26" s="44"/>
-      <c r="AL26" s="44"/>
-      <c r="AM26" s="44"/>
-      <c r="AN26" s="5"/>
+      <c r="A26" s="42"/>
+      <c r="B26" s="43"/>
+      <c r="C26" s="43"/>
+      <c r="D26" s="43"/>
+      <c r="E26" s="43"/>
+      <c r="F26" s="43"/>
+      <c r="G26" s="43"/>
+      <c r="H26" s="43"/>
+      <c r="I26" s="43"/>
+      <c r="J26" s="43"/>
+      <c r="K26" s="43"/>
+      <c r="L26" s="43"/>
+      <c r="M26" s="43"/>
+      <c r="N26" s="43"/>
+      <c r="O26" s="43"/>
+      <c r="P26" s="43"/>
+      <c r="Q26" s="44"/>
+      <c r="R26" s="21"/>
+      <c r="S26" s="21"/>
+      <c r="T26" s="21"/>
+      <c r="U26" s="21"/>
+      <c r="V26" s="21"/>
+      <c r="W26" s="21"/>
+      <c r="X26" s="21"/>
+      <c r="Y26" s="21"/>
+      <c r="Z26" s="21"/>
+      <c r="AA26" s="21"/>
+      <c r="AB26" s="21"/>
+      <c r="AC26" s="21"/>
+      <c r="AD26" s="21"/>
+      <c r="AE26" s="21"/>
+      <c r="AF26" s="21"/>
+      <c r="AG26" s="21"/>
+      <c r="AH26" s="21"/>
+      <c r="AI26" s="27"/>
+      <c r="AJ26" s="21"/>
+      <c r="AK26" s="21"/>
+      <c r="AL26" s="21"/>
+      <c r="AM26" s="21"/>
+      <c r="AN26" s="52"/>
+      <c r="AO26" s="52"/>
+      <c r="AP26" s="52"/>
+      <c r="AQ26" s="52"/>
+      <c r="AR26" s="52"/>
+      <c r="AS26" s="52"/>
+      <c r="AT26" s="52"/>
     </row>
   </sheetData>
   <mergeCells count="57">
-    <mergeCell ref="AK19:AT19"/>
-    <mergeCell ref="AK20:AT20"/>
-    <mergeCell ref="AK22:AL22"/>
-    <mergeCell ref="AM22:AT22"/>
-    <mergeCell ref="AK23:AT23"/>
     <mergeCell ref="AK24:AT24"/>
     <mergeCell ref="AK14:AL14"/>
     <mergeCell ref="AM14:AT14"/>
@@ -4370,11 +4546,11 @@
     <mergeCell ref="AK16:AT16"/>
     <mergeCell ref="AK18:AL18"/>
     <mergeCell ref="AM18:AT18"/>
-    <mergeCell ref="AK7:AT7"/>
-    <mergeCell ref="AK8:AT8"/>
-    <mergeCell ref="AK10:AL10"/>
-    <mergeCell ref="AM10:AT10"/>
-    <mergeCell ref="AK11:AT11"/>
+    <mergeCell ref="AK19:AT19"/>
+    <mergeCell ref="AK20:AT20"/>
+    <mergeCell ref="AK22:AL22"/>
+    <mergeCell ref="AM22:AT22"/>
+    <mergeCell ref="AK23:AT23"/>
     <mergeCell ref="AK12:AT12"/>
     <mergeCell ref="AK2:AL2"/>
     <mergeCell ref="AM2:AT2"/>
@@ -4382,16 +4558,21 @@
     <mergeCell ref="AK4:AT4"/>
     <mergeCell ref="AK6:AL6"/>
     <mergeCell ref="AM6:AT6"/>
+    <mergeCell ref="AK7:AT7"/>
+    <mergeCell ref="AK8:AT8"/>
+    <mergeCell ref="AK10:AL10"/>
+    <mergeCell ref="AM10:AT10"/>
+    <mergeCell ref="AK11:AT11"/>
+    <mergeCell ref="Y20:AH20"/>
+    <mergeCell ref="Y14:Z14"/>
+    <mergeCell ref="AA14:AH14"/>
+    <mergeCell ref="M23:V23"/>
+    <mergeCell ref="M24:V24"/>
     <mergeCell ref="Y15:AH15"/>
     <mergeCell ref="Y16:AH16"/>
     <mergeCell ref="Y18:Z18"/>
     <mergeCell ref="AA18:AH18"/>
     <mergeCell ref="Y19:AH19"/>
-    <mergeCell ref="Y20:AH20"/>
-    <mergeCell ref="Y14:Z14"/>
-    <mergeCell ref="AA14:AH14"/>
-    <mergeCell ref="M23:V23"/>
-    <mergeCell ref="M24:V24"/>
     <mergeCell ref="A25:Q26"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="C2:J2"/>
@@ -4416,7 +4597,8 @@
     <mergeCell ref="O10:V10"/>
     <mergeCell ref="M8:V8"/>
   </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.86614173228346458" right="0.86614173228346458" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
+  <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -4425,10 +4607,10 @@
   <sheetPr>
     <tabColor theme="0" tint="-0.249977111117893"/>
   </sheetPr>
-  <dimension ref="A1:AM26"/>
+  <dimension ref="A1:AT26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="R26" sqref="R26:AT27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="3.5703125" defaultRowHeight="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -4475,35 +4657,35 @@
       <c r="AJ1" s="4"/>
       <c r="AK1" s="4"/>
       <c r="AL1" s="4"/>
-      <c r="AM1" s="46"/>
+      <c r="AM1" s="4"/>
     </row>
     <row r="2" spans="1:39" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="8"/>
-      <c r="C2" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="D2" s="10"/>
-      <c r="E2" s="10"/>
-      <c r="F2" s="10"/>
-      <c r="G2" s="10"/>
-      <c r="H2" s="10"/>
-      <c r="I2" s="10"/>
-      <c r="J2" s="11"/>
+      <c r="B2" s="30"/>
+      <c r="C2" s="31" t="s">
+        <v>58</v>
+      </c>
+      <c r="D2" s="31"/>
+      <c r="E2" s="31"/>
+      <c r="F2" s="31"/>
+      <c r="G2" s="31"/>
+      <c r="H2" s="31"/>
+      <c r="I2" s="31"/>
+      <c r="J2" s="32"/>
       <c r="K2" s="2"/>
       <c r="L2" s="3"/>
-      <c r="M2" s="53"/>
-      <c r="N2" s="53"/>
-      <c r="O2" s="29"/>
-      <c r="P2" s="29"/>
-      <c r="Q2" s="29"/>
-      <c r="R2" s="29"/>
-      <c r="S2" s="29"/>
-      <c r="T2" s="29"/>
-      <c r="U2" s="29"/>
-      <c r="V2" s="29"/>
+      <c r="M2" s="28"/>
+      <c r="N2" s="28"/>
+      <c r="O2" s="12"/>
+      <c r="P2" s="12"/>
+      <c r="Q2" s="12"/>
+      <c r="R2" s="12"/>
+      <c r="S2" s="12"/>
+      <c r="T2" s="12"/>
+      <c r="U2" s="12"/>
+      <c r="V2" s="12"/>
       <c r="W2" s="3"/>
       <c r="X2" s="2"/>
       <c r="Y2" s="2"/>
@@ -4520,33 +4702,33 @@
       <c r="AJ2" s="2"/>
       <c r="AK2" s="2"/>
       <c r="AL2" s="2"/>
-      <c r="AM2" s="48"/>
+      <c r="AM2" s="2"/>
     </row>
     <row r="3" spans="1:39" ht="18.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="B3" s="15"/>
-      <c r="C3" s="15"/>
-      <c r="D3" s="15"/>
-      <c r="E3" s="15"/>
-      <c r="F3" s="15"/>
-      <c r="G3" s="15"/>
-      <c r="H3" s="15"/>
-      <c r="I3" s="15"/>
-      <c r="J3" s="16"/>
-      <c r="K3" s="51"/>
+      <c r="A3" s="33" t="s">
+        <v>59</v>
+      </c>
+      <c r="B3" s="34"/>
+      <c r="C3" s="34"/>
+      <c r="D3" s="34"/>
+      <c r="E3" s="34"/>
+      <c r="F3" s="34"/>
+      <c r="G3" s="34"/>
+      <c r="H3" s="34"/>
+      <c r="I3" s="34"/>
+      <c r="J3" s="35"/>
+      <c r="K3" s="26"/>
       <c r="L3" s="3"/>
-      <c r="M3" s="29"/>
-      <c r="N3" s="29"/>
-      <c r="O3" s="29"/>
-      <c r="P3" s="29"/>
-      <c r="Q3" s="29"/>
-      <c r="R3" s="29"/>
-      <c r="S3" s="29"/>
-      <c r="T3" s="29"/>
-      <c r="U3" s="29"/>
-      <c r="V3" s="29"/>
+      <c r="M3" s="12"/>
+      <c r="N3" s="12"/>
+      <c r="O3" s="12"/>
+      <c r="P3" s="12"/>
+      <c r="Q3" s="12"/>
+      <c r="R3" s="12"/>
+      <c r="S3" s="12"/>
+      <c r="T3" s="12"/>
+      <c r="U3" s="12"/>
+      <c r="V3" s="12"/>
       <c r="W3" s="3"/>
       <c r="X3" s="2"/>
       <c r="Y3" s="2"/>
@@ -4563,33 +4745,33 @@
       <c r="AJ3" s="2"/>
       <c r="AK3" s="2"/>
       <c r="AL3" s="2"/>
-      <c r="AM3" s="48"/>
+      <c r="AM3" s="2"/>
     </row>
     <row r="4" spans="1:39" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="22" t="s">
-        <v>15</v>
-      </c>
-      <c r="B4" s="23"/>
-      <c r="C4" s="23"/>
-      <c r="D4" s="23"/>
-      <c r="E4" s="23"/>
-      <c r="F4" s="23"/>
-      <c r="G4" s="23"/>
-      <c r="H4" s="23"/>
-      <c r="I4" s="23"/>
-      <c r="J4" s="24"/>
+      <c r="A4" s="36" t="s">
+        <v>60</v>
+      </c>
+      <c r="B4" s="37"/>
+      <c r="C4" s="37"/>
+      <c r="D4" s="37"/>
+      <c r="E4" s="37"/>
+      <c r="F4" s="37"/>
+      <c r="G4" s="37"/>
+      <c r="H4" s="37"/>
+      <c r="I4" s="37"/>
+      <c r="J4" s="38"/>
       <c r="K4" s="2"/>
       <c r="L4" s="3"/>
-      <c r="M4" s="29"/>
-      <c r="N4" s="29"/>
-      <c r="O4" s="29"/>
-      <c r="P4" s="29"/>
-      <c r="Q4" s="29"/>
-      <c r="R4" s="29"/>
-      <c r="S4" s="29"/>
-      <c r="T4" s="29"/>
-      <c r="U4" s="29"/>
-      <c r="V4" s="29"/>
+      <c r="M4" s="12"/>
+      <c r="N4" s="12"/>
+      <c r="O4" s="12"/>
+      <c r="P4" s="12"/>
+      <c r="Q4" s="12"/>
+      <c r="R4" s="12"/>
+      <c r="S4" s="12"/>
+      <c r="T4" s="12"/>
+      <c r="U4" s="12"/>
+      <c r="V4" s="12"/>
       <c r="W4" s="3"/>
       <c r="X4" s="2"/>
       <c r="Y4" s="2"/>
@@ -4606,18 +4788,18 @@
       <c r="AJ4" s="2"/>
       <c r="AK4" s="2"/>
       <c r="AL4" s="2"/>
-      <c r="AM4" s="48"/>
+      <c r="AM4" s="2"/>
     </row>
     <row r="5" spans="1:39" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="29"/>
-      <c r="B5" s="29"/>
-      <c r="C5" s="29"/>
-      <c r="D5" s="29"/>
-      <c r="E5" s="29"/>
-      <c r="F5" s="29"/>
-      <c r="G5" s="29"/>
-      <c r="H5" s="29"/>
-      <c r="I5" s="29"/>
+      <c r="A5" s="12"/>
+      <c r="B5" s="12"/>
+      <c r="C5" s="12"/>
+      <c r="D5" s="12"/>
+      <c r="E5" s="12"/>
+      <c r="F5" s="12"/>
+      <c r="G5" s="12"/>
+      <c r="H5" s="12"/>
+      <c r="I5" s="12"/>
       <c r="J5" s="2"/>
       <c r="K5" s="2"/>
       <c r="L5" s="3"/>
@@ -4647,7 +4829,7 @@
       <c r="AJ5" s="2"/>
       <c r="AK5" s="2"/>
       <c r="AL5" s="2"/>
-      <c r="AM5" s="48"/>
+      <c r="AM5" s="2"/>
     </row>
     <row r="6" spans="1:39" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
@@ -4688,7 +4870,7 @@
       <c r="AJ6" s="2"/>
       <c r="AK6" s="2"/>
       <c r="AL6" s="2"/>
-      <c r="AM6" s="48"/>
+      <c r="AM6" s="2"/>
     </row>
     <row r="7" spans="1:39" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
@@ -4729,7 +4911,7 @@
       <c r="AJ7" s="2"/>
       <c r="AK7" s="2"/>
       <c r="AL7" s="2"/>
-      <c r="AM7" s="48"/>
+      <c r="AM7" s="2"/>
     </row>
     <row r="8" spans="1:39" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
@@ -4770,7 +4952,7 @@
       <c r="AJ8" s="2"/>
       <c r="AK8" s="2"/>
       <c r="AL8" s="2"/>
-      <c r="AM8" s="48"/>
+      <c r="AM8" s="2"/>
     </row>
     <row r="9" spans="1:39" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="L9" s="3"/>
@@ -4800,20 +4982,20 @@
       <c r="AJ9" s="2"/>
       <c r="AK9" s="2"/>
       <c r="AL9" s="2"/>
-      <c r="AM9" s="48"/>
+      <c r="AM9" s="2"/>
     </row>
     <row r="10" spans="1:39" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="L10" s="3"/>
-      <c r="M10" s="53"/>
-      <c r="N10" s="53"/>
-      <c r="O10" s="29"/>
-      <c r="P10" s="29"/>
-      <c r="Q10" s="29"/>
-      <c r="R10" s="29"/>
-      <c r="S10" s="29"/>
-      <c r="T10" s="29"/>
-      <c r="U10" s="29"/>
-      <c r="V10" s="29"/>
+      <c r="M10" s="28"/>
+      <c r="N10" s="28"/>
+      <c r="O10" s="12"/>
+      <c r="P10" s="12"/>
+      <c r="Q10" s="12"/>
+      <c r="R10" s="12"/>
+      <c r="S10" s="12"/>
+      <c r="T10" s="12"/>
+      <c r="U10" s="12"/>
+      <c r="V10" s="12"/>
       <c r="W10" s="3"/>
       <c r="X10" s="2"/>
       <c r="Y10" s="2"/>
@@ -4830,20 +5012,20 @@
       <c r="AJ10" s="2"/>
       <c r="AK10" s="2"/>
       <c r="AL10" s="2"/>
-      <c r="AM10" s="48"/>
+      <c r="AM10" s="2"/>
     </row>
     <row r="11" spans="1:39" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="L11" s="3"/>
-      <c r="M11" s="29"/>
-      <c r="N11" s="29"/>
-      <c r="O11" s="29"/>
-      <c r="P11" s="29"/>
-      <c r="Q11" s="29"/>
-      <c r="R11" s="29"/>
-      <c r="S11" s="29"/>
-      <c r="T11" s="29"/>
-      <c r="U11" s="29"/>
-      <c r="V11" s="29"/>
+      <c r="M11" s="12"/>
+      <c r="N11" s="12"/>
+      <c r="O11" s="12"/>
+      <c r="P11" s="12"/>
+      <c r="Q11" s="12"/>
+      <c r="R11" s="12"/>
+      <c r="S11" s="12"/>
+      <c r="T11" s="12"/>
+      <c r="U11" s="12"/>
+      <c r="V11" s="12"/>
       <c r="W11" s="3"/>
       <c r="X11" s="2"/>
       <c r="Y11" s="2"/>
@@ -4860,20 +5042,20 @@
       <c r="AJ11" s="2"/>
       <c r="AK11" s="2"/>
       <c r="AL11" s="2"/>
-      <c r="AM11" s="48"/>
+      <c r="AM11" s="2"/>
     </row>
     <row r="12" spans="1:39" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="L12" s="3"/>
-      <c r="M12" s="29"/>
-      <c r="N12" s="29"/>
-      <c r="O12" s="29"/>
-      <c r="P12" s="29"/>
-      <c r="Q12" s="29"/>
-      <c r="R12" s="29"/>
-      <c r="S12" s="29"/>
-      <c r="T12" s="29"/>
-      <c r="U12" s="29"/>
-      <c r="V12" s="29"/>
+      <c r="M12" s="12"/>
+      <c r="N12" s="12"/>
+      <c r="O12" s="12"/>
+      <c r="P12" s="12"/>
+      <c r="Q12" s="12"/>
+      <c r="R12" s="12"/>
+      <c r="S12" s="12"/>
+      <c r="T12" s="12"/>
+      <c r="U12" s="12"/>
+      <c r="V12" s="12"/>
       <c r="W12" s="3"/>
       <c r="X12" s="2"/>
       <c r="Y12" s="2"/>
@@ -4890,7 +5072,7 @@
       <c r="AJ12" s="2"/>
       <c r="AK12" s="2"/>
       <c r="AL12" s="2"/>
-      <c r="AM12" s="48"/>
+      <c r="AM12" s="2"/>
     </row>
     <row r="13" spans="1:39" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="L13" s="3"/>
@@ -4920,18 +5102,18 @@
       <c r="AJ13" s="2"/>
       <c r="AK13" s="2"/>
       <c r="AL13" s="2"/>
-      <c r="AM13" s="48"/>
+      <c r="AM13" s="2"/>
     </row>
     <row r="14" spans="1:39" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="29"/>
-      <c r="B14" s="29"/>
-      <c r="C14" s="29"/>
-      <c r="D14" s="29"/>
-      <c r="E14" s="29"/>
-      <c r="F14" s="29"/>
-      <c r="G14" s="29"/>
-      <c r="H14" s="29"/>
-      <c r="I14" s="29"/>
+      <c r="A14" s="12"/>
+      <c r="B14" s="12"/>
+      <c r="C14" s="12"/>
+      <c r="D14" s="12"/>
+      <c r="E14" s="12"/>
+      <c r="F14" s="12"/>
+      <c r="G14" s="12"/>
+      <c r="H14" s="12"/>
+      <c r="I14" s="12"/>
       <c r="J14" s="2"/>
       <c r="K14" s="2"/>
       <c r="L14" s="3"/>
@@ -4961,15 +5143,15 @@
       <c r="AJ14" s="2"/>
       <c r="AK14" s="2"/>
       <c r="AL14" s="2"/>
-      <c r="AM14" s="48"/>
+      <c r="AM14" s="2"/>
     </row>
     <row r="15" spans="1:39" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="29"/>
-      <c r="B15" s="29"/>
-      <c r="C15" s="29"/>
-      <c r="D15" s="29"/>
-      <c r="E15" s="29"/>
-      <c r="F15" s="29"/>
+      <c r="A15" s="12"/>
+      <c r="B15" s="12"/>
+      <c r="C15" s="12"/>
+      <c r="D15" s="12"/>
+      <c r="E15" s="12"/>
+      <c r="F15" s="12"/>
       <c r="G15" s="3"/>
       <c r="H15" s="3"/>
       <c r="I15" s="2"/>
@@ -5002,7 +5184,7 @@
       <c r="AJ15" s="2"/>
       <c r="AK15" s="2"/>
       <c r="AL15" s="2"/>
-      <c r="AM15" s="48"/>
+      <c r="AM15" s="2"/>
     </row>
     <row r="16" spans="1:39" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
@@ -5043,9 +5225,9 @@
       <c r="AJ16" s="2"/>
       <c r="AK16" s="2"/>
       <c r="AL16" s="2"/>
-      <c r="AM16" s="48"/>
-    </row>
-    <row r="17" spans="1:39" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AM16" s="2"/>
+    </row>
+    <row r="17" spans="1:46" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
@@ -5084,9 +5266,9 @@
       <c r="AJ17" s="2"/>
       <c r="AK17" s="2"/>
       <c r="AL17" s="2"/>
-      <c r="AM17" s="48"/>
-    </row>
-    <row r="18" spans="1:39" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AM17" s="2"/>
+    </row>
+    <row r="18" spans="1:46" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
@@ -5099,16 +5281,16 @@
       <c r="J18" s="2"/>
       <c r="K18" s="2"/>
       <c r="L18" s="3"/>
-      <c r="M18" s="53"/>
-      <c r="N18" s="53"/>
-      <c r="O18" s="29"/>
-      <c r="P18" s="29"/>
-      <c r="Q18" s="29"/>
-      <c r="R18" s="29"/>
-      <c r="S18" s="29"/>
-      <c r="T18" s="29"/>
-      <c r="U18" s="29"/>
-      <c r="V18" s="29"/>
+      <c r="M18" s="28"/>
+      <c r="N18" s="28"/>
+      <c r="O18" s="12"/>
+      <c r="P18" s="12"/>
+      <c r="Q18" s="12"/>
+      <c r="R18" s="12"/>
+      <c r="S18" s="12"/>
+      <c r="T18" s="12"/>
+      <c r="U18" s="12"/>
+      <c r="V18" s="12"/>
       <c r="W18" s="3"/>
       <c r="X18" s="2"/>
       <c r="Y18" s="2"/>
@@ -5125,9 +5307,9 @@
       <c r="AJ18" s="2"/>
       <c r="AK18" s="2"/>
       <c r="AL18" s="2"/>
-      <c r="AM18" s="48"/>
-    </row>
-    <row r="19" spans="1:39" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AM18" s="2"/>
+    </row>
+    <row r="19" spans="1:46" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
@@ -5140,16 +5322,16 @@
       <c r="J19" s="2"/>
       <c r="K19" s="2"/>
       <c r="L19" s="3"/>
-      <c r="M19" s="29"/>
-      <c r="N19" s="29"/>
-      <c r="O19" s="29"/>
-      <c r="P19" s="29"/>
-      <c r="Q19" s="29"/>
-      <c r="R19" s="29"/>
-      <c r="S19" s="29"/>
-      <c r="T19" s="29"/>
-      <c r="U19" s="29"/>
-      <c r="V19" s="29"/>
+      <c r="M19" s="12"/>
+      <c r="N19" s="12"/>
+      <c r="O19" s="12"/>
+      <c r="P19" s="12"/>
+      <c r="Q19" s="12"/>
+      <c r="R19" s="12"/>
+      <c r="S19" s="12"/>
+      <c r="T19" s="12"/>
+      <c r="U19" s="12"/>
+      <c r="V19" s="12"/>
       <c r="W19" s="3"/>
       <c r="X19" s="2"/>
       <c r="Y19" s="2"/>
@@ -5166,9 +5348,9 @@
       <c r="AJ19" s="2"/>
       <c r="AK19" s="2"/>
       <c r="AL19" s="2"/>
-      <c r="AM19" s="48"/>
-    </row>
-    <row r="20" spans="1:39" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AM19" s="2"/>
+    </row>
+    <row r="20" spans="1:46" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
@@ -5181,16 +5363,16 @@
       <c r="J20" s="2"/>
       <c r="K20" s="2"/>
       <c r="L20" s="3"/>
-      <c r="M20" s="29"/>
-      <c r="N20" s="29"/>
-      <c r="O20" s="29"/>
-      <c r="P20" s="29"/>
-      <c r="Q20" s="29"/>
-      <c r="R20" s="29"/>
-      <c r="S20" s="29"/>
-      <c r="T20" s="29"/>
-      <c r="U20" s="29"/>
-      <c r="V20" s="29"/>
+      <c r="M20" s="12"/>
+      <c r="N20" s="12"/>
+      <c r="O20" s="12"/>
+      <c r="P20" s="12"/>
+      <c r="Q20" s="12"/>
+      <c r="R20" s="12"/>
+      <c r="S20" s="12"/>
+      <c r="T20" s="12"/>
+      <c r="U20" s="12"/>
+      <c r="V20" s="12"/>
       <c r="W20" s="3"/>
       <c r="X20" s="2"/>
       <c r="Y20" s="2"/>
@@ -5207,9 +5389,9 @@
       <c r="AJ20" s="2"/>
       <c r="AK20" s="2"/>
       <c r="AL20" s="2"/>
-      <c r="AM20" s="48"/>
-    </row>
-    <row r="21" spans="1:39" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AM20" s="2"/>
+    </row>
+    <row r="21" spans="1:46" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
@@ -5248,9 +5430,9 @@
       <c r="AJ21" s="2"/>
       <c r="AK21" s="2"/>
       <c r="AL21" s="2"/>
-      <c r="AM21" s="48"/>
-    </row>
-    <row r="22" spans="1:39" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AM21" s="2"/>
+    </row>
+    <row r="22" spans="1:46" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
@@ -5289,9 +5471,9 @@
       <c r="AJ22" s="2"/>
       <c r="AK22" s="2"/>
       <c r="AL22" s="2"/>
-      <c r="AM22" s="48"/>
-    </row>
-    <row r="23" spans="1:39" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AM22" s="2"/>
+    </row>
+    <row r="23" spans="1:46" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
@@ -5330,9 +5512,9 @@
       <c r="AJ23" s="2"/>
       <c r="AK23" s="2"/>
       <c r="AL23" s="2"/>
-      <c r="AM23" s="48"/>
-    </row>
-    <row r="24" spans="1:39" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AM23" s="2"/>
+    </row>
+    <row r="24" spans="1:46" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="1"/>
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
@@ -5371,28 +5553,28 @@
       <c r="AJ24" s="2"/>
       <c r="AK24" s="2"/>
       <c r="AL24" s="2"/>
-      <c r="AM24" s="48"/>
-    </row>
-    <row r="25" spans="1:39" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="38" t="s">
-        <v>16</v>
-      </c>
-      <c r="B25" s="39"/>
-      <c r="C25" s="39"/>
-      <c r="D25" s="39"/>
-      <c r="E25" s="39"/>
-      <c r="F25" s="39"/>
-      <c r="G25" s="39"/>
-      <c r="H25" s="39"/>
-      <c r="I25" s="39"/>
-      <c r="J25" s="39"/>
-      <c r="K25" s="39"/>
-      <c r="L25" s="39"/>
-      <c r="M25" s="39"/>
-      <c r="N25" s="39"/>
-      <c r="O25" s="39"/>
-      <c r="P25" s="39"/>
-      <c r="Q25" s="40"/>
+      <c r="AM24" s="2"/>
+    </row>
+    <row r="25" spans="1:46" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="39" t="s">
+        <v>13</v>
+      </c>
+      <c r="B25" s="40"/>
+      <c r="C25" s="40"/>
+      <c r="D25" s="40"/>
+      <c r="E25" s="40"/>
+      <c r="F25" s="40"/>
+      <c r="G25" s="40"/>
+      <c r="H25" s="40"/>
+      <c r="I25" s="40"/>
+      <c r="J25" s="40"/>
+      <c r="K25" s="40"/>
+      <c r="L25" s="40"/>
+      <c r="M25" s="40"/>
+      <c r="N25" s="40"/>
+      <c r="O25" s="40"/>
+      <c r="P25" s="40"/>
+      <c r="Q25" s="41"/>
       <c r="R25" s="2"/>
       <c r="S25" s="2"/>
       <c r="T25" s="2"/>
@@ -5414,48 +5596,55 @@
       <c r="AJ25" s="2"/>
       <c r="AK25" s="2"/>
       <c r="AL25" s="2"/>
-      <c r="AM25" s="48"/>
-    </row>
-    <row r="26" spans="1:39" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="41"/>
-      <c r="B26" s="42"/>
-      <c r="C26" s="42"/>
-      <c r="D26" s="42"/>
-      <c r="E26" s="42"/>
-      <c r="F26" s="42"/>
-      <c r="G26" s="42"/>
-      <c r="H26" s="42"/>
-      <c r="I26" s="42"/>
-      <c r="J26" s="42"/>
-      <c r="K26" s="42"/>
-      <c r="L26" s="42"/>
-      <c r="M26" s="42"/>
-      <c r="N26" s="42"/>
-      <c r="O26" s="42"/>
-      <c r="P26" s="42"/>
-      <c r="Q26" s="43"/>
-      <c r="R26" s="44"/>
-      <c r="S26" s="44"/>
-      <c r="T26" s="44"/>
-      <c r="U26" s="44"/>
-      <c r="V26" s="44"/>
-      <c r="W26" s="44"/>
-      <c r="X26" s="44"/>
-      <c r="Y26" s="44"/>
-      <c r="Z26" s="44"/>
-      <c r="AA26" s="44"/>
-      <c r="AB26" s="44"/>
-      <c r="AC26" s="44"/>
-      <c r="AD26" s="44"/>
-      <c r="AE26" s="44"/>
-      <c r="AF26" s="44"/>
-      <c r="AG26" s="44"/>
-      <c r="AH26" s="44"/>
-      <c r="AI26" s="44"/>
-      <c r="AJ26" s="44"/>
-      <c r="AK26" s="44"/>
-      <c r="AL26" s="44"/>
-      <c r="AM26" s="52"/>
+      <c r="AM25" s="2"/>
+    </row>
+    <row r="26" spans="1:46" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="42"/>
+      <c r="B26" s="43"/>
+      <c r="C26" s="43"/>
+      <c r="D26" s="43"/>
+      <c r="E26" s="43"/>
+      <c r="F26" s="43"/>
+      <c r="G26" s="43"/>
+      <c r="H26" s="43"/>
+      <c r="I26" s="43"/>
+      <c r="J26" s="43"/>
+      <c r="K26" s="43"/>
+      <c r="L26" s="43"/>
+      <c r="M26" s="43"/>
+      <c r="N26" s="43"/>
+      <c r="O26" s="43"/>
+      <c r="P26" s="43"/>
+      <c r="Q26" s="44"/>
+      <c r="R26" s="21"/>
+      <c r="S26" s="21"/>
+      <c r="T26" s="21"/>
+      <c r="U26" s="21"/>
+      <c r="V26" s="21"/>
+      <c r="W26" s="21"/>
+      <c r="X26" s="21"/>
+      <c r="Y26" s="21"/>
+      <c r="Z26" s="21"/>
+      <c r="AA26" s="21"/>
+      <c r="AB26" s="21"/>
+      <c r="AC26" s="21"/>
+      <c r="AD26" s="21"/>
+      <c r="AE26" s="21"/>
+      <c r="AF26" s="21"/>
+      <c r="AG26" s="21"/>
+      <c r="AH26" s="21"/>
+      <c r="AI26" s="27"/>
+      <c r="AJ26" s="21"/>
+      <c r="AK26" s="21"/>
+      <c r="AL26" s="21"/>
+      <c r="AM26" s="21"/>
+      <c r="AN26" s="52"/>
+      <c r="AO26" s="52"/>
+      <c r="AP26" s="52"/>
+      <c r="AQ26" s="52"/>
+      <c r="AR26" s="52"/>
+      <c r="AS26" s="52"/>
+      <c r="AT26" s="52"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -5465,6 +5654,7 @@
     <mergeCell ref="A3:J3"/>
     <mergeCell ref="A4:J4"/>
   </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.86614173228346458" right="0.86614173228346458" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
+  <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>